<commit_message>
seizure detection agent summary and chart
</commit_message>
<xml_diff>
--- a/china/seizures/pangolin-seizures.xlsx
+++ b/china/seizures/pangolin-seizures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tangruibin/Documents/Pangolin/china/seizures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D125A80B-7BD2-BA40-A793-E57D9AFB6817}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29C6901-9B34-704D-9CE0-55A57854EDCE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4934" uniqueCount="2031">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4934" uniqueCount="2030">
   <si>
     <t>Year</t>
   </si>
@@ -5807,11 +5807,6 @@
   </si>
   <si>
     <t>Neijiang</t>
-  </si>
-  <si>
-    <t>Market 
-Supervision 
-Administration</t>
   </si>
   <si>
     <t>张君秋：10months, 1year</t>
@@ -6835,7 +6830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -7227,6 +7222,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7546,9 +7544,9 @@
   </sheetPr>
   <dimension ref="A1:AS992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -10064,7 +10062,7 @@
       <c r="AR27" s="36"/>
       <c r="AS27" s="36"/>
     </row>
-    <row r="28" spans="1:45" ht="19">
+    <row r="28" spans="1:45" ht="31">
       <c r="A28" s="7" t="s">
         <v>217</v>
       </c>
@@ -10083,7 +10081,7 @@
       <c r="F28" s="7" t="s">
         <v>1467</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G28" s="165" t="s">
         <v>1496</v>
       </c>
       <c r="H28" s="7" t="s">
@@ -16765,7 +16763,7 @@
       <c r="AR98" s="36"/>
       <c r="AS98" s="36"/>
     </row>
-    <row r="99" spans="1:45" ht="13">
+    <row r="99" spans="1:45" ht="42">
       <c r="A99" s="7" t="s">
         <v>153</v>
       </c>
@@ -16784,8 +16782,8 @@
       <c r="F99" s="7" t="s">
         <v>1823</v>
       </c>
-      <c r="G99" s="7" t="s">
-        <v>1824</v>
+      <c r="G99" s="25" t="s">
+        <v>343</v>
       </c>
       <c r="H99" s="41"/>
       <c r="I99" s="41"/>
@@ -16802,7 +16800,7 @@
         <v>360</v>
       </c>
       <c r="P99" s="43" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="Q99" s="7" t="s">
         <v>1594</v>
@@ -16820,7 +16818,7 @@
         <v>263</v>
       </c>
       <c r="V99" s="45" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="W99" s="41"/>
       <c r="X99" s="7" t="s">
@@ -16830,7 +16828,7 @@
         <v>102</v>
       </c>
       <c r="Z99" s="7" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="AA99" s="2" t="s">
         <v>116</v>
@@ -16884,7 +16882,7 @@
       <c r="I100" s="41"/>
       <c r="J100" s="41"/>
       <c r="K100" s="7" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="L100" s="41"/>
       <c r="M100" s="41"/>
@@ -16895,7 +16893,7 @@
         <v>360</v>
       </c>
       <c r="P100" s="43" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="Q100" s="7" t="s">
         <v>537</v>
@@ -16913,7 +16911,7 @@
         <v>263</v>
       </c>
       <c r="V100" s="45" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="W100" s="41"/>
       <c r="X100" s="7" t="s">
@@ -16929,7 +16927,7 @@
       </c>
       <c r="AE100" s="36"/>
       <c r="AF100" s="149" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="AG100" s="36"/>
       <c r="AH100" s="36"/>
@@ -16962,7 +16960,7 @@
         <v>452</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="G101" s="7" t="s">
         <v>418</v>
@@ -16976,7 +16974,7 @@
       <c r="N101" s="82"/>
       <c r="O101" s="41"/>
       <c r="P101" s="43" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="Q101" s="7" t="s">
         <v>1504</v>
@@ -16994,20 +16992,20 @@
         <v>263</v>
       </c>
       <c r="V101" s="45" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="W101" s="41"/>
       <c r="X101" s="150" t="s">
         <v>1765</v>
       </c>
       <c r="Y101" s="150" t="s">
+        <v>1834</v>
+      </c>
+      <c r="Z101" s="150" t="s">
         <v>1835</v>
       </c>
-      <c r="Z101" s="150" t="s">
+      <c r="AA101" s="151" t="s">
         <v>1836</v>
-      </c>
-      <c r="AA101" s="151" t="s">
-        <v>1837</v>
       </c>
       <c r="AB101" s="36"/>
       <c r="AC101" s="36"/>
@@ -17016,7 +17014,7 @@
       </c>
       <c r="AE101" s="36"/>
       <c r="AF101" s="2" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="AG101" s="36"/>
       <c r="AH101" s="36"/>
@@ -17042,7 +17040,7 @@
         <v>107</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="F102" s="41"/>
       <c r="G102" s="7" t="s">
@@ -17054,15 +17052,15 @@
       <c r="K102" s="41"/>
       <c r="L102" s="7"/>
       <c r="M102" s="7" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="N102" s="82"/>
       <c r="O102" s="41"/>
       <c r="P102" s="43" t="s">
+        <v>1840</v>
+      </c>
+      <c r="Q102" s="7" t="s">
         <v>1841</v>
-      </c>
-      <c r="Q102" s="7" t="s">
-        <v>1842</v>
       </c>
       <c r="R102" s="7" t="s">
         <v>360</v>
@@ -17077,14 +17075,14 @@
         <v>263</v>
       </c>
       <c r="V102" s="45" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="W102" s="41"/>
       <c r="X102" s="7" t="s">
         <v>101</v>
       </c>
       <c r="Y102" s="7" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="Z102" s="41"/>
       <c r="AA102" s="36"/>
@@ -17095,7 +17093,7 @@
       </c>
       <c r="AE102" s="36"/>
       <c r="AF102" s="2" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="AG102" s="36"/>
       <c r="AH102" s="36"/>
@@ -17131,16 +17129,16 @@
         <v>1592</v>
       </c>
       <c r="G103" s="7" t="s">
+        <v>1845</v>
+      </c>
+      <c r="H103" s="7" t="s">
         <v>1846</v>
       </c>
-      <c r="H103" s="7" t="s">
+      <c r="I103" s="7" t="s">
         <v>1847</v>
       </c>
-      <c r="I103" s="7" t="s">
+      <c r="J103" s="7" t="s">
         <v>1848</v>
-      </c>
-      <c r="J103" s="7" t="s">
-        <v>1849</v>
       </c>
       <c r="K103" s="41"/>
       <c r="L103" s="7" t="s">
@@ -17150,10 +17148,10 @@
       <c r="N103" s="82"/>
       <c r="O103" s="41"/>
       <c r="P103" s="43" t="s">
+        <v>1849</v>
+      </c>
+      <c r="Q103" s="7" t="s">
         <v>1850</v>
-      </c>
-      <c r="Q103" s="7" t="s">
-        <v>1851</v>
       </c>
       <c r="R103" s="7" t="s">
         <v>360</v>
@@ -17168,7 +17166,7 @@
         <v>263</v>
       </c>
       <c r="V103" s="45" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="W103" s="41"/>
       <c r="X103" s="7" t="s">
@@ -17176,7 +17174,7 @@
       </c>
       <c r="Y103" s="41"/>
       <c r="Z103" s="7" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="AA103" s="2" t="s">
         <v>50</v>
@@ -17218,10 +17216,10 @@
         <v>107</v>
       </c>
       <c r="E104" s="7" t="s">
+        <v>1853</v>
+      </c>
+      <c r="F104" s="7" t="s">
         <v>1854</v>
-      </c>
-      <c r="F104" s="7" t="s">
-        <v>1855</v>
       </c>
       <c r="G104" s="7" t="s">
         <v>418</v>
@@ -17233,20 +17231,20 @@
         <v>891</v>
       </c>
       <c r="J104" s="7" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="K104" s="41"/>
       <c r="L104" s="7" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="M104" s="41"/>
       <c r="N104" s="82"/>
       <c r="O104" s="41"/>
       <c r="P104" s="43" t="s">
+        <v>1857</v>
+      </c>
+      <c r="Q104" s="7" t="s">
         <v>1858</v>
-      </c>
-      <c r="Q104" s="7" t="s">
-        <v>1859</v>
       </c>
       <c r="R104" s="3" t="s">
         <v>360</v>
@@ -17261,7 +17259,7 @@
         <v>263</v>
       </c>
       <c r="V104" s="45" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="W104" s="41"/>
       <c r="X104" s="7" t="s">
@@ -17271,10 +17269,10 @@
         <v>273</v>
       </c>
       <c r="Z104" s="7" t="s">
+        <v>1860</v>
+      </c>
+      <c r="AA104" s="2" t="s">
         <v>1861</v>
-      </c>
-      <c r="AA104" s="2" t="s">
-        <v>1862</v>
       </c>
       <c r="AB104" s="36"/>
       <c r="AC104" s="36"/>
@@ -17334,7 +17332,7 @@
         <v>360</v>
       </c>
       <c r="P105" s="43" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="Q105" s="7" t="s">
         <v>1504</v>
@@ -17352,7 +17350,7 @@
         <v>263</v>
       </c>
       <c r="V105" s="45" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="W105" s="7" t="s">
         <v>1818</v>
@@ -17364,7 +17362,7 @@
         <v>102</v>
       </c>
       <c r="Z105" s="7" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="AA105" s="2" t="s">
         <v>1524</v>
@@ -17406,10 +17404,10 @@
         <v>107</v>
       </c>
       <c r="E106" s="7" t="s">
+        <v>1865</v>
+      </c>
+      <c r="F106" s="7" t="s">
         <v>1866</v>
-      </c>
-      <c r="F106" s="7" t="s">
-        <v>1867</v>
       </c>
       <c r="G106" s="7" t="s">
         <v>407</v>
@@ -17427,10 +17425,10 @@
         <v>360</v>
       </c>
       <c r="P106" s="43" t="s">
+        <v>1867</v>
+      </c>
+      <c r="Q106" s="7" t="s">
         <v>1868</v>
-      </c>
-      <c r="Q106" s="7" t="s">
-        <v>1869</v>
       </c>
       <c r="R106" s="3" t="s">
         <v>360</v>
@@ -17445,7 +17443,7 @@
         <v>263</v>
       </c>
       <c r="V106" s="45" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="W106" s="41"/>
       <c r="X106" s="7" t="s">
@@ -17469,7 +17467,7 @@
       </c>
       <c r="AE106" s="36"/>
       <c r="AF106" s="2" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="AG106" s="36"/>
       <c r="AH106" s="36"/>
@@ -17522,7 +17520,7 @@
         <v>360</v>
       </c>
       <c r="P107" s="43" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="Q107" s="7" t="s">
         <v>1504</v>
@@ -17540,7 +17538,7 @@
         <v>263</v>
       </c>
       <c r="V107" s="45" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="W107" s="41"/>
       <c r="X107" s="7" t="s">
@@ -17566,7 +17564,7 @@
       </c>
       <c r="AE107" s="36"/>
       <c r="AF107" s="2" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="AG107" s="36"/>
       <c r="AH107" s="36"/>
@@ -17599,7 +17597,7 @@
         <v>452</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="G108" s="7" t="s">
         <v>45</v>
@@ -17613,7 +17611,7 @@
       <c r="N108" s="82"/>
       <c r="O108" s="41"/>
       <c r="P108" s="43" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="Q108" s="7" t="s">
         <v>458</v>
@@ -17631,7 +17629,7 @@
         <v>263</v>
       </c>
       <c r="V108" s="45" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="W108" s="7" t="s">
         <v>179</v>
@@ -17700,16 +17698,16 @@
       </c>
       <c r="K109" s="41"/>
       <c r="L109" s="7" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="M109" s="7"/>
       <c r="N109" s="82"/>
       <c r="O109" s="41"/>
       <c r="P109" s="43" t="s">
+        <v>1878</v>
+      </c>
+      <c r="Q109" s="7" t="s">
         <v>1879</v>
-      </c>
-      <c r="Q109" s="7" t="s">
-        <v>1880</v>
       </c>
       <c r="R109" s="3" t="s">
         <v>360</v>
@@ -17724,7 +17722,7 @@
         <v>263</v>
       </c>
       <c r="V109" s="45" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="W109" s="7" t="s">
         <v>1818</v>
@@ -17733,13 +17731,13 @@
         <v>1788</v>
       </c>
       <c r="Y109" s="7" t="s">
+        <v>1881</v>
+      </c>
+      <c r="Z109" s="7" t="s">
         <v>1882</v>
       </c>
-      <c r="Z109" s="7" t="s">
+      <c r="AA109" s="2" t="s">
         <v>1883</v>
-      </c>
-      <c r="AA109" s="2" t="s">
-        <v>1884</v>
       </c>
       <c r="AB109" s="36"/>
       <c r="AC109" s="36"/>
@@ -17781,7 +17779,7 @@
         <v>881</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="G110" s="7" t="s">
         <v>418</v>
@@ -17794,21 +17792,21 @@
         <v>1695</v>
       </c>
       <c r="M110" s="7" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="N110" s="82"/>
       <c r="O110" s="41"/>
       <c r="P110" s="138" t="s">
+        <v>1886</v>
+      </c>
+      <c r="Q110" s="7" t="s">
         <v>1887</v>
-      </c>
-      <c r="Q110" s="7" t="s">
-        <v>1888</v>
       </c>
       <c r="R110" s="3" t="s">
         <v>360</v>
       </c>
       <c r="S110" s="7" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="T110" s="20" t="s">
         <v>107</v>
@@ -17817,18 +17815,18 @@
         <v>263</v>
       </c>
       <c r="V110" s="45" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="W110" s="41"/>
       <c r="X110" s="7" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="Y110" s="41"/>
       <c r="Z110" s="7" t="s">
         <v>1685</v>
       </c>
       <c r="AA110" s="2" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="AB110" s="36"/>
       <c r="AC110" s="36"/>
@@ -17837,7 +17835,7 @@
       </c>
       <c r="AE110" s="36"/>
       <c r="AF110" s="2" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="AG110" s="36"/>
       <c r="AH110" s="36"/>
@@ -17884,7 +17882,7 @@
       <c r="N111" s="82"/>
       <c r="O111" s="41"/>
       <c r="P111" s="43" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="Q111" s="7" t="s">
         <v>1504</v>
@@ -17902,7 +17900,7 @@
         <v>263</v>
       </c>
       <c r="V111" s="45" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="W111" s="7" t="s">
         <v>179</v>
@@ -17915,7 +17913,7 @@
         <v>1685</v>
       </c>
       <c r="AA111" s="2" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="AB111" s="36"/>
       <c r="AC111" s="36"/>
@@ -17968,15 +17966,15 @@
       <c r="K112" s="41"/>
       <c r="L112" s="41"/>
       <c r="M112" s="7" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="N112" s="82"/>
       <c r="O112" s="41"/>
       <c r="P112" s="43" t="s">
+        <v>1895</v>
+      </c>
+      <c r="Q112" s="7" t="s">
         <v>1896</v>
-      </c>
-      <c r="Q112" s="7" t="s">
-        <v>1897</v>
       </c>
       <c r="R112" s="3" t="s">
         <v>360</v>
@@ -17991,7 +17989,7 @@
         <v>263</v>
       </c>
       <c r="V112" s="45" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="W112" s="41"/>
       <c r="X112" s="7" t="s">
@@ -18001,7 +17999,7 @@
         <v>102</v>
       </c>
       <c r="Z112" s="100" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="AA112" s="2" t="s">
         <v>49</v>
@@ -18013,7 +18011,7 @@
       </c>
       <c r="AE112" s="36"/>
       <c r="AF112" s="2" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="AG112" s="36"/>
       <c r="AH112" s="36"/>
@@ -18066,7 +18064,7 @@
         <v>360</v>
       </c>
       <c r="P113" s="43" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="Q113" s="7" t="s">
         <v>1594</v>
@@ -18084,7 +18082,7 @@
         <v>263</v>
       </c>
       <c r="V113" s="45" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="W113" s="41"/>
       <c r="X113" s="7" t="s">
@@ -18094,7 +18092,7 @@
         <v>102</v>
       </c>
       <c r="Z113" s="7" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="AA113" s="2" t="s">
         <v>1524</v>
@@ -18161,7 +18159,7 @@
         <v>360</v>
       </c>
       <c r="P114" s="43" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="Q114" s="7" t="s">
         <v>458</v>
@@ -18179,7 +18177,7 @@
         <v>263</v>
       </c>
       <c r="V114" s="45" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="W114" s="7" t="s">
         <v>1818</v>
@@ -18191,7 +18189,7 @@
         <v>102</v>
       </c>
       <c r="Z114" s="7" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="AA114" s="2" t="s">
         <v>49</v>
@@ -18240,7 +18238,7 @@
         <v>1597</v>
       </c>
       <c r="F115" s="7" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="G115" s="7" t="s">
         <v>407</v>
@@ -18258,7 +18256,7 @@
         <v>360</v>
       </c>
       <c r="P115" s="43" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="Q115" s="7" t="s">
         <v>458</v>
@@ -18276,7 +18274,7 @@
         <v>263</v>
       </c>
       <c r="V115" s="45" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="W115" s="41"/>
       <c r="X115" s="7" t="s">
@@ -18298,7 +18296,7 @@
       </c>
       <c r="AE115" s="36"/>
       <c r="AF115" s="2" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="AG115" s="36"/>
       <c r="AH115" s="36"/>
@@ -18349,7 +18347,7 @@
         <v>360</v>
       </c>
       <c r="P116" s="43" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="Q116" s="7" t="s">
         <v>537</v>
@@ -18367,7 +18365,7 @@
         <v>263</v>
       </c>
       <c r="V116" s="45" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="W116" s="7" t="s">
         <v>1818</v>
@@ -18379,7 +18377,7 @@
         <v>102</v>
       </c>
       <c r="Z116" s="7" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="AA116" s="2" t="s">
         <v>116</v>
@@ -18395,7 +18393,7 @@
       </c>
       <c r="AE116" s="36"/>
       <c r="AF116" s="2" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="AG116" s="36"/>
       <c r="AH116" s="36"/>
@@ -18439,12 +18437,12 @@
       <c r="K117" s="41"/>
       <c r="L117" s="41"/>
       <c r="M117" s="7" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="N117" s="82"/>
       <c r="O117" s="41"/>
       <c r="P117" s="43" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="Q117" s="7" t="s">
         <v>368</v>
@@ -18462,7 +18460,7 @@
         <v>263</v>
       </c>
       <c r="V117" s="45" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="W117" s="41"/>
       <c r="X117" s="7" t="s">
@@ -18472,10 +18470,10 @@
         <v>273</v>
       </c>
       <c r="Z117" s="7" t="s">
+        <v>1916</v>
+      </c>
+      <c r="AA117" s="2" t="s">
         <v>1917</v>
-      </c>
-      <c r="AA117" s="2" t="s">
-        <v>1918</v>
       </c>
       <c r="AB117" s="36"/>
       <c r="AC117" s="36"/>
@@ -18517,7 +18515,7 @@
         <v>429</v>
       </c>
       <c r="F118" s="7" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="G118" s="7" t="s">
         <v>431</v>
@@ -18537,7 +18535,7 @@
         <v>360</v>
       </c>
       <c r="P118" s="43" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="Q118" s="7" t="s">
         <v>1594</v>
@@ -18555,7 +18553,7 @@
         <v>263</v>
       </c>
       <c r="V118" s="45" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="W118" s="7" t="s">
         <v>1818</v>
@@ -18581,7 +18579,7 @@
       </c>
       <c r="AE118" s="36"/>
       <c r="AF118" s="2" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="AG118" s="36"/>
       <c r="AH118" s="36"/>
@@ -18610,7 +18608,7 @@
         <v>334</v>
       </c>
       <c r="F119" s="101" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="G119" s="101" t="s">
         <v>418</v>
@@ -18638,20 +18636,20 @@
         <v>263</v>
       </c>
       <c r="V119" s="118" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="W119" s="102"/>
       <c r="X119" s="101" t="s">
+        <v>1924</v>
+      </c>
+      <c r="Y119" s="101" t="s">
+        <v>1881</v>
+      </c>
+      <c r="Z119" s="101" t="s">
         <v>1925</v>
       </c>
-      <c r="Y119" s="101" t="s">
-        <v>1882</v>
-      </c>
-      <c r="Z119" s="101" t="s">
+      <c r="AA119" s="108" t="s">
         <v>1926</v>
-      </c>
-      <c r="AA119" s="108" t="s">
-        <v>1927</v>
       </c>
       <c r="AB119" s="108">
         <v>8016</v>
@@ -18664,7 +18662,7 @@
       </c>
       <c r="AE119" s="109"/>
       <c r="AF119" s="108" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="AG119" s="109"/>
       <c r="AH119" s="109"/>
@@ -18697,7 +18695,7 @@
         <v>429</v>
       </c>
       <c r="F120" s="7" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="G120" s="7" t="s">
         <v>418</v>
@@ -18721,7 +18719,7 @@
         <v>360</v>
       </c>
       <c r="P120" s="43" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="Q120" s="7" t="s">
         <v>1504</v>
@@ -18739,23 +18737,23 @@
         <v>263</v>
       </c>
       <c r="V120" s="45" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="W120" s="41"/>
       <c r="X120" s="7" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="Y120" s="7" t="s">
         <v>1766</v>
       </c>
       <c r="Z120" s="7" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="AA120" s="2" t="s">
         <v>1820</v>
       </c>
       <c r="AB120" s="2" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="AC120" s="2" t="s">
         <v>360</v>
@@ -18765,7 +18763,7 @@
       </c>
       <c r="AE120" s="36"/>
       <c r="AF120" s="2" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="AG120" s="36"/>
       <c r="AH120" s="36"/>
@@ -18809,7 +18807,7 @@
       <c r="K121" s="41"/>
       <c r="L121" s="41"/>
       <c r="M121" s="7" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="N121" s="42">
         <v>1670</v>
@@ -18818,10 +18816,10 @@
         <v>360</v>
       </c>
       <c r="P121" s="43" t="s">
+        <v>1935</v>
+      </c>
+      <c r="Q121" s="7" t="s">
         <v>1936</v>
-      </c>
-      <c r="Q121" s="7" t="s">
-        <v>1937</v>
       </c>
       <c r="R121" s="3" t="s">
         <v>360</v>
@@ -18836,7 +18834,7 @@
         <v>263</v>
       </c>
       <c r="V121" s="45" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="W121" s="7" t="s">
         <v>1818</v>
@@ -18848,7 +18846,7 @@
         <v>273</v>
       </c>
       <c r="Z121" s="7" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="AA121" s="2" t="s">
         <v>116</v>
@@ -18911,7 +18909,7 @@
       <c r="N122" s="82"/>
       <c r="O122" s="41"/>
       <c r="P122" s="43" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="Q122" s="7" t="s">
         <v>458</v>
@@ -18929,7 +18927,7 @@
         <v>263</v>
       </c>
       <c r="V122" s="45" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="W122" s="41"/>
       <c r="X122" s="7" t="s">
@@ -18937,7 +18935,7 @@
       </c>
       <c r="Y122" s="41"/>
       <c r="Z122" s="7" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="AA122" s="2" t="s">
         <v>50</v>
@@ -19000,7 +18998,7 @@
         <v>360</v>
       </c>
       <c r="P123" s="43" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="Q123" s="7" t="s">
         <v>1504</v>
@@ -19018,7 +19016,7 @@
         <v>263</v>
       </c>
       <c r="V123" s="45" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="W123" s="7" t="s">
         <v>1493</v>
@@ -19030,7 +19028,7 @@
         <v>102</v>
       </c>
       <c r="Z123" s="7" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="AA123" s="2" t="s">
         <v>49</v>
@@ -19099,10 +19097,10 @@
       <c r="N124" s="82"/>
       <c r="O124" s="41"/>
       <c r="P124" s="43" t="s">
+        <v>1945</v>
+      </c>
+      <c r="Q124" s="7" t="s">
         <v>1946</v>
-      </c>
-      <c r="Q124" s="7" t="s">
-        <v>1947</v>
       </c>
       <c r="R124" s="3" t="s">
         <v>360</v>
@@ -19117,7 +19115,7 @@
         <v>263</v>
       </c>
       <c r="V124" s="45" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="W124" s="41"/>
       <c r="X124" s="7" t="s">
@@ -19184,7 +19182,7 @@
       <c r="N125" s="82"/>
       <c r="O125" s="41"/>
       <c r="P125" s="43" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="Q125" s="7" t="s">
         <v>1504</v>
@@ -19202,7 +19200,7 @@
         <v>263</v>
       </c>
       <c r="V125" s="45" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="W125" s="41"/>
       <c r="X125" s="7" t="s">
@@ -19212,7 +19210,7 @@
         <v>102</v>
       </c>
       <c r="Z125" s="7" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="AA125" s="2" t="s">
         <v>116</v>
@@ -19224,7 +19222,7 @@
       </c>
       <c r="AE125" s="36"/>
       <c r="AF125" s="2" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="AG125" s="36"/>
       <c r="AH125" s="36"/>
@@ -19257,31 +19255,31 @@
         <v>421</v>
       </c>
       <c r="F126" s="7" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="G126" s="7" t="s">
         <v>418</v>
       </c>
       <c r="H126" s="7" t="s">
+        <v>1953</v>
+      </c>
+      <c r="I126" s="7" t="s">
         <v>1954</v>
       </c>
-      <c r="I126" s="7" t="s">
+      <c r="J126" s="7" t="s">
         <v>1955</v>
-      </c>
-      <c r="J126" s="7" t="s">
-        <v>1956</v>
       </c>
       <c r="K126" s="41"/>
       <c r="L126" s="7" t="s">
         <v>1695</v>
       </c>
       <c r="M126" s="7" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="N126" s="82"/>
       <c r="O126" s="41"/>
       <c r="P126" s="43" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="Q126" s="7" t="s">
         <v>458</v>
@@ -19299,7 +19297,7 @@
         <v>263</v>
       </c>
       <c r="V126" s="45" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="W126" s="41"/>
       <c r="X126" s="7" t="s">
@@ -19309,10 +19307,10 @@
         <v>102</v>
       </c>
       <c r="Z126" s="7" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="AA126" s="2" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="AB126" s="36"/>
       <c r="AC126" s="36"/>
@@ -19372,7 +19370,7 @@
         <v>360</v>
       </c>
       <c r="P127" s="125" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="Q127" s="122" t="s">
         <v>424</v>
@@ -19390,19 +19388,19 @@
         <v>263</v>
       </c>
       <c r="V127" s="127" t="s">
+        <v>1961</v>
+      </c>
+      <c r="W127" s="122" t="s">
         <v>1962</v>
-      </c>
-      <c r="W127" s="122" t="s">
-        <v>1963</v>
       </c>
       <c r="X127" s="122" t="s">
         <v>412</v>
       </c>
       <c r="Y127" s="122" t="s">
+        <v>1963</v>
+      </c>
+      <c r="Z127" s="122" t="s">
         <v>1964</v>
-      </c>
-      <c r="Z127" s="122" t="s">
-        <v>1965</v>
       </c>
       <c r="AA127" s="129" t="s">
         <v>50</v>
@@ -19414,7 +19412,7 @@
       </c>
       <c r="AE127" s="130"/>
       <c r="AF127" s="129" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="AG127" s="130"/>
       <c r="AH127" s="130"/>
@@ -19447,7 +19445,7 @@
         <v>452</v>
       </c>
       <c r="F128" s="122" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="G128" s="122" t="s">
         <v>418</v>
@@ -19465,7 +19463,7 @@
         <v>360</v>
       </c>
       <c r="P128" s="125" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="Q128" s="122" t="s">
         <v>1808</v>
@@ -19483,17 +19481,17 @@
         <v>263</v>
       </c>
       <c r="V128" s="127" t="s">
+        <v>1961</v>
+      </c>
+      <c r="W128" s="122" t="s">
         <v>1962</v>
       </c>
-      <c r="W128" s="122" t="s">
-        <v>1963</v>
-      </c>
       <c r="X128" s="122" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="Y128" s="123"/>
       <c r="Z128" s="122" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="AA128" s="129" t="s">
         <v>50</v>
@@ -19505,7 +19503,7 @@
       </c>
       <c r="AE128" s="130"/>
       <c r="AF128" s="129" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="AG128" s="130"/>
       <c r="AH128" s="130"/>
@@ -19538,7 +19536,7 @@
         <v>429</v>
       </c>
       <c r="F129" s="7" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="G129" s="7" t="s">
         <v>407</v>
@@ -19549,7 +19547,7 @@
       <c r="K129" s="41"/>
       <c r="L129" s="41"/>
       <c r="M129" s="7" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="N129" s="2">
         <v>4186</v>
@@ -19558,7 +19556,7 @@
         <v>360</v>
       </c>
       <c r="P129" s="43" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="Q129" s="7" t="s">
         <v>1594</v>
@@ -19576,7 +19574,7 @@
         <v>263</v>
       </c>
       <c r="V129" s="45" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="W129" s="41"/>
       <c r="X129" s="7" t="s">
@@ -19586,7 +19584,7 @@
         <v>102</v>
       </c>
       <c r="Z129" s="7" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="AA129" s="2" t="s">
         <v>49</v>
@@ -19646,7 +19644,7 @@
       <c r="K130" s="41"/>
       <c r="L130" s="41"/>
       <c r="M130" s="7" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="N130" s="42">
         <v>2182</v>
@@ -19655,7 +19653,7 @@
         <v>360</v>
       </c>
       <c r="P130" s="43" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="Q130" s="7" t="s">
         <v>1778</v>
@@ -19673,7 +19671,7 @@
         <v>263</v>
       </c>
       <c r="V130" s="45" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="W130" s="41"/>
       <c r="X130" s="7" t="s">
@@ -19683,7 +19681,7 @@
         <v>102</v>
       </c>
       <c r="Z130" s="7" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="AA130" s="2" t="s">
         <v>49</v>
@@ -19743,7 +19741,7 @@
       <c r="K131" s="41"/>
       <c r="L131" s="41"/>
       <c r="M131" s="7" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="N131" s="42">
         <v>5229</v>
@@ -19752,7 +19750,7 @@
         <v>360</v>
       </c>
       <c r="P131" s="43" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="Q131" s="7" t="s">
         <v>368</v>
@@ -19770,7 +19768,7 @@
         <v>263</v>
       </c>
       <c r="V131" s="45" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="W131" s="41"/>
       <c r="X131" s="7" t="s">
@@ -19780,7 +19778,7 @@
         <v>102</v>
       </c>
       <c r="Z131" s="7" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="AA131" s="2" t="s">
         <v>49</v>
@@ -19840,7 +19838,7 @@
       <c r="K132" s="41"/>
       <c r="L132" s="41"/>
       <c r="M132" s="7" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="N132" s="42">
         <v>4141</v>
@@ -19849,7 +19847,7 @@
         <v>360</v>
       </c>
       <c r="P132" s="43" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="Q132" s="7" t="s">
         <v>1594</v>
@@ -19867,7 +19865,7 @@
         <v>263</v>
       </c>
       <c r="V132" s="45" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="W132" s="41"/>
       <c r="X132" s="7" t="s">
@@ -19877,7 +19875,7 @@
         <v>102</v>
       </c>
       <c r="Z132" s="7" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="AA132" s="2" t="s">
         <v>49</v>
@@ -19926,7 +19924,7 @@
         <v>334</v>
       </c>
       <c r="F133" s="122" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="G133" s="122" t="s">
         <v>418</v>
@@ -19944,16 +19942,16 @@
         <v>360</v>
       </c>
       <c r="P133" s="125" t="s">
+        <v>1983</v>
+      </c>
+      <c r="Q133" s="122" t="s">
         <v>1984</v>
-      </c>
-      <c r="Q133" s="122" t="s">
-        <v>1985</v>
       </c>
       <c r="R133" s="157" t="s">
         <v>360</v>
       </c>
       <c r="S133" s="122" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="T133" s="126" t="s">
         <v>107</v>
@@ -19962,7 +19960,7 @@
         <v>263</v>
       </c>
       <c r="V133" s="127" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="W133" s="123"/>
       <c r="X133" s="122" t="s">
@@ -19970,7 +19968,7 @@
       </c>
       <c r="Y133" s="123"/>
       <c r="Z133" s="122" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="AA133" s="129" t="s">
         <v>50</v>
@@ -19982,7 +19980,7 @@
       </c>
       <c r="AE133" s="130"/>
       <c r="AF133" s="129" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="AG133" s="130"/>
       <c r="AH133" s="130"/>
@@ -20033,16 +20031,16 @@
         <v>360</v>
       </c>
       <c r="P134" s="125" t="s">
+        <v>1988</v>
+      </c>
+      <c r="Q134" s="122" t="s">
         <v>1989</v>
-      </c>
-      <c r="Q134" s="122" t="s">
-        <v>1990</v>
       </c>
       <c r="R134" s="157" t="s">
         <v>360</v>
       </c>
       <c r="S134" s="122" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="T134" s="126" t="s">
         <v>107</v>
@@ -20051,7 +20049,7 @@
         <v>263</v>
       </c>
       <c r="V134" s="122" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="W134" s="123"/>
       <c r="X134" s="122" t="s">
@@ -20071,7 +20069,7 @@
       </c>
       <c r="AE134" s="130"/>
       <c r="AF134" s="129" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="AG134" s="130"/>
       <c r="AH134" s="130"/>
@@ -20122,16 +20120,16 @@
         <v>360</v>
       </c>
       <c r="P135" s="125" t="s">
+        <v>1991</v>
+      </c>
+      <c r="Q135" s="122" t="s">
         <v>1992</v>
-      </c>
-      <c r="Q135" s="122" t="s">
-        <v>1993</v>
       </c>
       <c r="R135" s="157" t="s">
         <v>360</v>
       </c>
       <c r="S135" s="122" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="T135" s="126" t="s">
         <v>107</v>
@@ -20140,7 +20138,7 @@
         <v>263</v>
       </c>
       <c r="V135" s="122" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="W135" s="123"/>
       <c r="X135" s="122" t="s">
@@ -20148,7 +20146,7 @@
       </c>
       <c r="Y135" s="123"/>
       <c r="Z135" s="122" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="AA135" s="129" t="s">
         <v>50</v>
@@ -20197,7 +20195,7 @@
         <v>334</v>
       </c>
       <c r="F136" s="122" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="G136" s="122" t="s">
         <v>418</v>
@@ -20215,16 +20213,16 @@
         <v>360</v>
       </c>
       <c r="P136" s="125" t="s">
+        <v>1995</v>
+      </c>
+      <c r="Q136" s="122" t="s">
         <v>1996</v>
-      </c>
-      <c r="Q136" s="122" t="s">
-        <v>1997</v>
       </c>
       <c r="R136" s="157" t="s">
         <v>360</v>
       </c>
       <c r="S136" s="122" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="T136" s="126" t="s">
         <v>107</v>
@@ -20233,20 +20231,20 @@
         <v>263</v>
       </c>
       <c r="V136" s="122" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="W136" s="123"/>
       <c r="X136" s="122" t="s">
+        <v>1998</v>
+      </c>
+      <c r="Y136" s="122" t="s">
         <v>1999</v>
       </c>
-      <c r="Y136" s="122" t="s">
+      <c r="Z136" s="122" t="s">
         <v>2000</v>
       </c>
-      <c r="Z136" s="122" t="s">
+      <c r="AA136" s="129" t="s">
         <v>2001</v>
-      </c>
-      <c r="AA136" s="129" t="s">
-        <v>2002</v>
       </c>
       <c r="AB136" s="130"/>
       <c r="AC136" s="130"/>
@@ -20255,7 +20253,7 @@
       </c>
       <c r="AE136" s="130"/>
       <c r="AF136" s="129" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="AG136" s="130"/>
       <c r="AH136" s="130"/>
@@ -20302,7 +20300,7 @@
       <c r="N137" s="135"/>
       <c r="O137" s="123"/>
       <c r="P137" s="125" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="Q137" s="122" t="s">
         <v>424</v>
@@ -20311,7 +20309,7 @@
         <v>360</v>
       </c>
       <c r="S137" s="122" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="T137" s="126" t="s">
         <v>107</v>
@@ -20320,7 +20318,7 @@
         <v>263</v>
       </c>
       <c r="V137" s="122" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="W137" s="123"/>
       <c r="X137" s="122" t="s">
@@ -20333,7 +20331,7 @@
         <v>170</v>
       </c>
       <c r="AA137" s="129" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="AB137" s="130"/>
       <c r="AC137" s="130"/>
@@ -20375,7 +20373,7 @@
         <v>334</v>
       </c>
       <c r="F138" s="122" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="G138" s="122" t="s">
         <v>418</v>
@@ -20386,7 +20384,7 @@
       <c r="K138" s="123"/>
       <c r="L138" s="123"/>
       <c r="M138" s="122" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="N138" s="129">
         <v>534</v>
@@ -20395,7 +20393,7 @@
         <v>360</v>
       </c>
       <c r="P138" s="125" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="Q138" s="122" t="s">
         <v>424</v>
@@ -20404,7 +20402,7 @@
         <v>360</v>
       </c>
       <c r="S138" s="122" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="T138" s="126" t="s">
         <v>107</v>
@@ -20413,20 +20411,20 @@
         <v>263</v>
       </c>
       <c r="V138" s="122" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="W138" s="123"/>
       <c r="X138" s="122" t="s">
         <v>101</v>
       </c>
       <c r="Y138" s="122" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="Z138" s="122" t="s">
         <v>1685</v>
       </c>
       <c r="AA138" s="129" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="AB138" s="129">
         <v>534</v>
@@ -20472,7 +20470,7 @@
         <v>334</v>
       </c>
       <c r="F139" s="122" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="G139" s="122" t="s">
         <v>418</v>
@@ -20483,12 +20481,12 @@
       <c r="K139" s="123"/>
       <c r="L139" s="123"/>
       <c r="M139" s="122" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="N139" s="135"/>
       <c r="O139" s="123"/>
       <c r="P139" s="125" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="Q139" s="122" t="s">
         <v>424</v>
@@ -20497,7 +20495,7 @@
         <v>360</v>
       </c>
       <c r="S139" s="122" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="T139" s="126" t="s">
         <v>107</v>
@@ -20506,7 +20504,7 @@
         <v>263</v>
       </c>
       <c r="V139" s="122" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="W139" s="123"/>
       <c r="X139" s="122" t="s">
@@ -20561,24 +20559,24 @@
         <v>1437</v>
       </c>
       <c r="F140" s="7" t="s">
+        <v>2011</v>
+      </c>
+      <c r="G140" s="7" t="s">
         <v>2012</v>
       </c>
-      <c r="G140" s="7" t="s">
+      <c r="H140" s="7" t="s">
         <v>2013</v>
       </c>
-      <c r="H140" s="7" t="s">
+      <c r="I140" s="7" t="s">
         <v>2014</v>
       </c>
-      <c r="I140" s="7" t="s">
+      <c r="J140" s="7" t="s">
         <v>2015</v>
-      </c>
-      <c r="J140" s="7" t="s">
-        <v>2016</v>
       </c>
       <c r="K140" s="41"/>
       <c r="L140" s="41"/>
       <c r="M140" s="7" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="N140" s="82"/>
       <c r="O140" s="41"/>
@@ -20597,7 +20595,7 @@
         <v>263</v>
       </c>
       <c r="V140" s="45" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="W140" s="41"/>
       <c r="X140" s="7" t="s">
@@ -20650,19 +20648,19 @@
         <v>452</v>
       </c>
       <c r="F141" s="7" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="G141" s="7" t="s">
         <v>407</v>
       </c>
       <c r="H141" s="7" t="s">
+        <v>2018</v>
+      </c>
+      <c r="I141" s="7" t="s">
         <v>2019</v>
       </c>
-      <c r="I141" s="7" t="s">
+      <c r="J141" s="7" t="s">
         <v>2020</v>
-      </c>
-      <c r="J141" s="7" t="s">
-        <v>2021</v>
       </c>
       <c r="K141" s="41"/>
       <c r="L141" s="7" t="s">
@@ -20686,7 +20684,7 @@
         <v>263</v>
       </c>
       <c r="V141" s="45" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="W141" s="41"/>
       <c r="X141" s="7" t="s">
@@ -20694,7 +20692,7 @@
       </c>
       <c r="Y141" s="41"/>
       <c r="Z141" s="7" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="AA141" s="2" t="s">
         <v>50</v>
@@ -20737,10 +20735,10 @@
         <v>334</v>
       </c>
       <c r="F142" s="7" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="G142" s="7" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="H142" s="41"/>
       <c r="I142" s="41"/>
@@ -20765,7 +20763,7 @@
         <v>263</v>
       </c>
       <c r="V142" s="45" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="W142" s="41"/>
       <c r="X142" s="7" t="s">
@@ -20775,7 +20773,7 @@
         <v>102</v>
       </c>
       <c r="Z142" s="7" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="AA142" s="2" t="s">
         <v>49</v>
@@ -20823,14 +20821,14 @@
         <v>1336</v>
       </c>
       <c r="G143" s="7" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="H143" s="41"/>
       <c r="I143" s="41"/>
       <c r="J143" s="41"/>
       <c r="K143" s="41"/>
       <c r="L143" s="7" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="M143" s="41"/>
       <c r="N143" s="42">
@@ -20854,7 +20852,7 @@
         <v>263</v>
       </c>
       <c r="V143" s="45" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="W143" s="41"/>
       <c r="X143" s="7" t="s">
@@ -20876,7 +20874,7 @@
       </c>
       <c r="AE143" s="36"/>
       <c r="AF143" s="2" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="AG143" s="36"/>
       <c r="AH143" s="36"/>
@@ -20947,7 +20945,7 @@
         <v>263</v>
       </c>
       <c r="V144" s="45" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="W144" s="41"/>
       <c r="X144" s="7" t="s">
@@ -20957,7 +20955,7 @@
         <v>102</v>
       </c>
       <c r="Z144" s="7" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="AA144" s="2" t="s">
         <v>116</v>
@@ -21036,7 +21034,7 @@
         <v>263</v>
       </c>
       <c r="V145" s="45" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="W145" s="41"/>
       <c r="X145" s="7" t="s">

</xml_diff>

<commit_message>
normalise court case incidances, plot all 388 cases
</commit_message>
<xml_diff>
--- a/china/seizures/pangolin-seizures.xlsx
+++ b/china/seizures/pangolin-seizures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tangruibin/Documents/Pangolin/china/seizures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29C6901-9B34-704D-9CE0-55A57854EDCE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6C4A03-E4FE-2842-8F6F-AC3420CA7AD0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7544,8 +7544,8 @@
   </sheetPr>
   <dimension ref="A1:AS992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update seizure data and visuals
</commit_message>
<xml_diff>
--- a/china/seizures/pangolin-seizures.xlsx
+++ b/china/seizures/pangolin-seizures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tangruibin/Documents/Pangolin/china/seizures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D663E099-5806-8E4F-95F2-DCDF36B5D3E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2020AA26-6A18-D448-9002-4940B8AA636E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6060" yWindow="1480" windowWidth="29580" windowHeight="18280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data table" sheetId="1" r:id="rId1"/>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4928" uniqueCount="2021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5237" uniqueCount="2091">
   <si>
     <t>Year</t>
   </si>
@@ -6526,6 +6526,218 @@
 龙某某：1y and 2mon
 马某某：6mon,1y</t>
   </si>
+  <si>
+    <t>Zhuhai</t>
+  </si>
+  <si>
+    <t>International waters near Malaysia</t>
+  </si>
+  <si>
+    <t>Jiangmen, Guangdong</t>
+  </si>
+  <si>
+    <t>Zhuhai, Guangdong</t>
+  </si>
+  <si>
+    <t>ship</t>
+  </si>
+  <si>
+    <t>罗桂基</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=4efa5c6b-3a05-479d-8f73-2d3199462463&amp;area=0&amp;index=1&amp;sortType=1&amp;count=4&amp;conditions=searchWord%2B%E7%BD%97%E6%A1%82%E5%9F%BA%2B1%2B%E7%BD%97%E6%A1%82%E5%9F%BA</t>
+  </si>
+  <si>
+    <t>Lincang</t>
+  </si>
+  <si>
+    <t>Wa State, Mayanmar</t>
+  </si>
+  <si>
+    <t>Lincang, Yunnan, China</t>
+  </si>
+  <si>
+    <t>鲍文杰</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=f1dd42a3-8e14-4a59-ae91-027232b86184&amp;area=0&amp;index=9&amp;sortType=2&amp;count=20&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2019%2B7%2B2019</t>
+  </si>
+  <si>
+    <t>2019-04-08 mainly drugs</t>
+  </si>
+  <si>
+    <t>Zhongshan</t>
+  </si>
+  <si>
+    <t>TongChung, HongKong</t>
+  </si>
+  <si>
+    <t>Zhongshan, Guangdong</t>
+  </si>
+  <si>
+    <t>motorboat</t>
+  </si>
+  <si>
+    <t>冼健强</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=af840564-ec8a-4674-8f78-2243a65f3310&amp;area=0&amp;index=5&amp;sortType=2&amp;count=20&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2019%2B7%2B2019</t>
+  </si>
+  <si>
+    <t>Lweje, Myanmar</t>
+  </si>
+  <si>
+    <t>Dehongzhou,Yunnan, China</t>
+  </si>
+  <si>
+    <t>张某某</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=0f816eb5-7e64-4b2f-a4c3-a65eefcdb33c&amp;area=0&amp;index=119&amp;sortType=2&amp;count=120&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2018%2B7%2B2018</t>
+  </si>
+  <si>
+    <t>勐赛, Myanmar</t>
+  </si>
+  <si>
+    <t>Xishuangbanna, Yunnan, China</t>
+  </si>
+  <si>
+    <t>van and logistics</t>
+  </si>
+  <si>
+    <t>陈洪波</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=370b1547-85ae-4d83-ad1e-8c05e3380bd4&amp;area=0&amp;index=100&amp;sortType=2&amp;count=120&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2018%2B7%2B2018</t>
+  </si>
+  <si>
+    <t>mainly other wildlife</t>
+  </si>
+  <si>
+    <t>王军亿</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=a94a9e50-0d56-4017-b1cb-e154aa783369&amp;area=0&amp;index=94&amp;sortType=2&amp;count=120&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2018%2B7%2B2018</t>
+  </si>
+  <si>
+    <t>mainly 檀香紫檀，合计总价1841，400元</t>
+  </si>
+  <si>
+    <t>Shanghai, China</t>
+  </si>
+  <si>
+    <t>container</t>
+  </si>
+  <si>
+    <t>朱凌云</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=95a5f1f7-17e3-4273-9bc8-e5d5198a359c&amp;area=0&amp;index=92&amp;sortType=2&amp;count=120&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2018%2B7%2B2018</t>
+  </si>
+  <si>
+    <t>Beihai</t>
+  </si>
+  <si>
+    <t>Guangzhou; Shenzheng; Zhuhai</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=b0fed416-ebf4-49a1-9a1a-8845bbb34e37&amp;area=0&amp;index=87&amp;sortType=2&amp;count=120&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2018%2B7%2B2018</t>
+  </si>
+  <si>
+    <t>公诉机关指控，2013年11月27日至2014年4月2日期间，被告人林中在越南组织2295只穿山甲</t>
+  </si>
+  <si>
+    <t>Addis Ababa, Ethiopia</t>
+  </si>
+  <si>
+    <t>Guangzhou, Guangdong</t>
+  </si>
+  <si>
+    <t>air</t>
+  </si>
+  <si>
+    <t>徐飞、汪付云、徐为林</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=56658deb-0901-4c3c-b0f2-f37098878b5b&amp;area=0&amp;index=78&amp;sortType=2&amp;count=120&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2018%2B7%2B2018</t>
+  </si>
+  <si>
+    <t>Manistricuspis</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=750edd50-d798-4804-b1f8-24c7ae107c33&amp;area=0&amp;index=16&amp;sortType=2&amp;count=120&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2018%2B7%2B2018</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Korea; HongKong; Shenzheng, Guangdong, China</t>
+  </si>
+  <si>
+    <t>Foshan, Guangdong, China</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=1f94f63e-146b-4715-9c9d-d704126c8506&amp;area=0&amp;index=3&amp;sortType=2&amp;count=120&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2018%2B7%2B2018</t>
+  </si>
+  <si>
+    <t>Phataginus tricuspis
+Manis pentadactyla</t>
+  </si>
+  <si>
+    <t>Myitkyina, Myanmar</t>
+  </si>
+  <si>
+    <t>Tengchong,Yunnan</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=56172897-68e4-4a17-85f7-c845792aa1f3&amp;area=0&amp;index=100&amp;sortType=2&amp;count=101&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2017%2B7%2B2017</t>
+  </si>
+  <si>
+    <t>Manentadactyla</t>
+  </si>
+  <si>
+    <t>Mongla, Myanmar</t>
+  </si>
+  <si>
+    <t>Xishuangbanna, Yunnan</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=97dc8373-005f-42e3-a988-ef582e54ce9a&amp;area=0&amp;index=98&amp;sortType=2&amp;count=101&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2017%2B7%2B2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2
+</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=b573442b-55b0-4f2c-9b75-e17faa4c2dd1&amp;area=0&amp;index=68&amp;sortType=2&amp;count=101&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2017%2B7%2B2017</t>
+  </si>
+  <si>
+    <t>Pangwa, Myanmar</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=914deead-897f-4324-8665-929402616f0f&amp;area=0&amp;index=47&amp;sortType=2&amp;count=101&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2017%2B7%2B2017</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=479efecc-6f48-4072-81cb-db013c515105&amp;area=0&amp;index=41&amp;sortType=2&amp;count=101&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2017%2B7%2B2017</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=a3c83d7d-4184-4a8c-8ecc-8118b1c9d5c6&amp;area=0&amp;index=28&amp;sortType=2&amp;count=101&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2017%2B7%2B2017</t>
+  </si>
+  <si>
+    <t>including other</t>
+  </si>
+  <si>
+    <t>Tibet</t>
+  </si>
+  <si>
+    <t>Shigatse</t>
+  </si>
+  <si>
+    <t>https://www.itslaw.com/detail?judgementId=b387494a-27c4-44d2-8f87-bc3f9226a67f&amp;area=0&amp;index=18&amp;sortType=2&amp;count=101&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2017%2B7%2B2017</t>
+  </si>
+  <si>
+    <t>brought from Nepalese</t>
+  </si>
 </sst>
 </file>
 
@@ -6536,7 +6748,7 @@
     <numFmt numFmtId="165" formatCode="#,##0;\(#,##0\)"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="34">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -6707,6 +6919,32 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="PingFang SC"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -6830,10 +7068,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -7219,13 +7458,6 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -7244,8 +7476,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7563,9 +7812,9 @@
   </sheetPr>
   <dimension ref="A1:AS992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB120" sqref="AB120"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F147" sqref="F147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -7581,7 +7830,7 @@
     <col min="20" max="20" width="21.83203125" customWidth="1"/>
     <col min="24" max="24" width="20.83203125" customWidth="1"/>
     <col min="27" max="27" width="15.1640625" customWidth="1"/>
-    <col min="28" max="28" width="14.5" style="168"/>
+    <col min="28" max="28" width="14.5" style="163"/>
     <col min="32" max="32" width="94.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7667,7 +7916,7 @@
       <c r="AA1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" s="168" t="s">
+      <c r="AB1" s="163" t="s">
         <v>35</v>
       </c>
       <c r="AC1" s="2" t="s">
@@ -7766,7 +8015,7 @@
       <c r="AA2" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="AB2" s="168">
+      <c r="AB2" s="163">
         <v>1035</v>
       </c>
       <c r="AC2" s="31" t="s">
@@ -8047,7 +8296,7 @@
       <c r="AA5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB5" s="168">
+      <c r="AB5" s="163">
         <v>1357120</v>
       </c>
       <c r="AC5" s="2" t="s">
@@ -8148,7 +8397,7 @@
       <c r="AA6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB6" s="168">
+      <c r="AB6" s="163">
         <v>9506</v>
       </c>
       <c r="AC6" s="2" t="s">
@@ -8243,7 +8492,7 @@
       <c r="AA7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AB7" s="168">
+      <c r="AB7" s="163">
         <v>26720</v>
       </c>
       <c r="AC7" s="2" t="s">
@@ -8588,7 +8837,7 @@
         <v>37</v>
       </c>
       <c r="AA11" s="65"/>
-      <c r="AB11" s="168">
+      <c r="AB11" s="163">
         <v>89020</v>
       </c>
       <c r="AC11" s="66" t="s">
@@ -8767,7 +9016,7 @@
         <v>1084</v>
       </c>
       <c r="AA13" s="54"/>
-      <c r="AB13" s="168">
+      <c r="AB13" s="163">
         <v>50000</v>
       </c>
       <c r="AC13" s="55" t="s">
@@ -8856,7 +9105,7 @@
         <v>170</v>
       </c>
       <c r="AA14" s="54"/>
-      <c r="AB14" s="168">
+      <c r="AB14" s="163">
         <v>9800</v>
       </c>
       <c r="AC14" s="55" t="s">
@@ -8949,7 +9198,7 @@
         <v>1099</v>
       </c>
       <c r="AA15" s="54"/>
-      <c r="AB15" s="168">
+      <c r="AB15" s="163">
         <v>272210</v>
       </c>
       <c r="AC15" s="55" t="s">
@@ -9128,7 +9377,7 @@
         <v>1115</v>
       </c>
       <c r="AA17" s="54"/>
-      <c r="AB17" s="168">
+      <c r="AB17" s="163">
         <v>66800</v>
       </c>
       <c r="AC17" s="55" t="s">
@@ -9217,7 +9466,7 @@
         <v>1155</v>
       </c>
       <c r="AA18" s="54"/>
-      <c r="AB18" s="168">
+      <c r="AB18" s="163">
         <v>172010</v>
       </c>
       <c r="AC18" s="55" t="s">
@@ -9308,7 +9557,7 @@
         <v>331</v>
       </c>
       <c r="AA19" s="54"/>
-      <c r="AB19" s="168">
+      <c r="AB19" s="163">
         <v>25384</v>
       </c>
       <c r="AC19" s="55" t="s">
@@ -9399,7 +9648,7 @@
         <v>1260</v>
       </c>
       <c r="AA20" s="54"/>
-      <c r="AB20" s="168">
+      <c r="AB20" s="163">
         <v>70140</v>
       </c>
       <c r="AC20" s="55" t="s">
@@ -9860,7 +10109,7 @@
       <c r="AA25" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AB25" s="168">
+      <c r="AB25" s="163">
         <v>32000</v>
       </c>
       <c r="AC25" s="2" t="s">
@@ -9885,7 +10134,7 @@
       <c r="AR25" s="35"/>
       <c r="AS25" s="35"/>
     </row>
-    <row r="26" spans="1:45" ht="14">
+    <row r="26" spans="1:45" ht="28">
       <c r="A26" s="100" t="s">
         <v>217</v>
       </c>
@@ -9897,7 +10146,7 @@
       <c r="E26" s="100" t="s">
         <v>1474</v>
       </c>
-      <c r="F26" s="164" t="s">
+      <c r="F26" s="159" t="s">
         <v>1475</v>
       </c>
       <c r="G26" s="102" t="s">
@@ -9954,7 +10203,7 @@
         <v>404</v>
       </c>
       <c r="AE26" s="108"/>
-      <c r="AF26" s="165" t="s">
+      <c r="AF26" s="160" t="s">
         <v>2001</v>
       </c>
       <c r="AG26" s="108"/>
@@ -10043,7 +10292,7 @@
       <c r="AA27" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AB27" s="168" t="s">
+      <c r="AB27" s="163" t="s">
         <v>1490</v>
       </c>
       <c r="AC27" s="7" t="s">
@@ -10146,7 +10395,7 @@
       <c r="AA28" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AB28" s="168">
+      <c r="AB28" s="163">
         <v>32000</v>
       </c>
       <c r="AC28" s="112" t="s">
@@ -10273,7 +10522,7 @@
       <c r="AR29" s="35"/>
       <c r="AS29" s="35"/>
     </row>
-    <row r="30" spans="1:45" ht="15">
+    <row r="30" spans="1:45" ht="29">
       <c r="A30" s="7" t="s">
         <v>217</v>
       </c>
@@ -10433,7 +10682,7 @@
       <c r="AA31" s="107" t="s">
         <v>116</v>
       </c>
-      <c r="AB31" s="168">
+      <c r="AB31" s="163">
         <v>5888</v>
       </c>
       <c r="AC31" s="118" t="s">
@@ -10548,7 +10797,7 @@
       <c r="AR32" s="35"/>
       <c r="AS32" s="35"/>
     </row>
-    <row r="33" spans="1:45" ht="13">
+    <row r="33" spans="1:45" ht="42">
       <c r="A33" s="7" t="s">
         <v>217</v>
       </c>
@@ -10720,7 +10969,7 @@
       <c r="AA34" s="66" t="s">
         <v>1518</v>
       </c>
-      <c r="AB34" s="168">
+      <c r="AB34" s="163">
         <v>2756.5</v>
       </c>
       <c r="AC34" s="66" t="s">
@@ -10825,7 +11074,7 @@
       <c r="AA35" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="AB35" s="168">
+      <c r="AB35" s="163">
         <v>12024</v>
       </c>
       <c r="AC35" s="66" t="s">
@@ -10922,7 +11171,7 @@
       <c r="AA36" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB36" s="168">
+      <c r="AB36" s="163">
         <v>2940</v>
       </c>
       <c r="AC36" s="2" t="s">
@@ -11201,7 +11450,7 @@
       <c r="AA39" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AB39" s="168">
+      <c r="AB39" s="163">
         <v>32000</v>
       </c>
       <c r="AC39" s="7" t="s">
@@ -11228,7 +11477,7 @@
       <c r="AR39" s="35"/>
       <c r="AS39" s="35"/>
     </row>
-    <row r="40" spans="1:45" ht="14">
+    <row r="40" spans="1:45" ht="42">
       <c r="A40" s="120" t="s">
         <v>153</v>
       </c>
@@ -11314,7 +11563,7 @@
       <c r="AR40" s="128"/>
       <c r="AS40" s="128"/>
     </row>
-    <row r="41" spans="1:45" ht="14">
+    <row r="41" spans="1:45" ht="42">
       <c r="A41" s="120" t="s">
         <v>153</v>
       </c>
@@ -11474,7 +11723,7 @@
       <c r="AA42" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AB42" s="168">
+      <c r="AB42" s="163">
         <v>40000</v>
       </c>
       <c r="AC42" s="2" t="s">
@@ -11573,7 +11822,7 @@
       <c r="AA43" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB43" s="168">
+      <c r="AB43" s="163">
         <v>32000</v>
       </c>
       <c r="AC43" s="2" t="s">
@@ -11600,7 +11849,7 @@
       <c r="AR43" s="35"/>
       <c r="AS43" s="35"/>
     </row>
-    <row r="44" spans="1:45" ht="13">
+    <row r="44" spans="1:45" ht="112">
       <c r="A44" s="100" t="s">
         <v>217</v>
       </c>
@@ -11626,7 +11875,7 @@
       </c>
       <c r="N44" s="103"/>
       <c r="O44" s="101"/>
-      <c r="P44" s="164" t="s">
+      <c r="P44" s="159" t="s">
         <v>1560</v>
       </c>
       <c r="Q44" s="100" t="s">
@@ -11663,7 +11912,7 @@
         <v>404</v>
       </c>
       <c r="AE44" s="108"/>
-      <c r="AF44" s="165" t="s">
+      <c r="AF44" s="160" t="s">
         <v>1564</v>
       </c>
       <c r="AG44" s="108"/>
@@ -11752,7 +12001,7 @@
       <c r="AA45" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB45" s="168">
+      <c r="AB45" s="163">
         <v>32000</v>
       </c>
       <c r="AC45" s="2" t="s">
@@ -12111,7 +12360,7 @@
       <c r="AA49" s="2" t="s">
         <v>1518</v>
       </c>
-      <c r="AB49" s="168">
+      <c r="AB49" s="163">
         <v>405</v>
       </c>
       <c r="AC49" s="7" t="s">
@@ -12138,7 +12387,7 @@
       <c r="AR49" s="35"/>
       <c r="AS49" s="35"/>
     </row>
-    <row r="50" spans="1:45" ht="14">
+    <row r="50" spans="1:45" ht="42">
       <c r="A50" s="138" t="s">
         <v>153</v>
       </c>
@@ -12174,7 +12423,7 @@
       <c r="O50" s="138" t="s">
         <v>360</v>
       </c>
-      <c r="P50" s="166" t="s">
+      <c r="P50" s="161" t="s">
         <v>1592</v>
       </c>
       <c r="Q50" s="138" t="s">
@@ -12208,7 +12457,7 @@
       <c r="AA50" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="AB50" s="168">
+      <c r="AB50" s="163">
         <v>668</v>
       </c>
       <c r="AC50" s="138" t="s">
@@ -12309,7 +12558,7 @@
       <c r="AA51" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB51" s="168">
+      <c r="AB51" s="163">
         <v>32000</v>
       </c>
       <c r="AC51" s="2" t="s">
@@ -12428,7 +12677,7 @@
       <c r="AR52" s="35"/>
       <c r="AS52" s="35"/>
     </row>
-    <row r="53" spans="1:45" ht="13">
+    <row r="53" spans="1:45" ht="28">
       <c r="A53" s="120" t="s">
         <v>153</v>
       </c>
@@ -12496,7 +12745,7 @@
       <c r="AA53" s="127" t="s">
         <v>50</v>
       </c>
-      <c r="AB53" s="168">
+      <c r="AB53" s="163">
         <v>1670</v>
       </c>
       <c r="AC53" s="127" t="s">
@@ -12523,7 +12772,7 @@
       <c r="AR53" s="128"/>
       <c r="AS53" s="128"/>
     </row>
-    <row r="54" spans="1:45" ht="13">
+    <row r="54" spans="1:45" ht="28">
       <c r="A54" s="120" t="s">
         <v>153</v>
       </c>
@@ -12593,7 +12842,7 @@
       <c r="AA54" s="127" t="s">
         <v>116</v>
       </c>
-      <c r="AB54" s="168">
+      <c r="AB54" s="163">
         <v>18704</v>
       </c>
       <c r="AC54" s="127" t="s">
@@ -12694,7 +12943,7 @@
       <c r="AA55" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AB55" s="168">
+      <c r="AB55" s="163">
         <v>2712.4</v>
       </c>
       <c r="AC55" s="2" t="s">
@@ -12889,7 +13138,7 @@
       <c r="AA57" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AB57" s="168">
+      <c r="AB57" s="163">
         <v>3340</v>
       </c>
       <c r="AC57" s="2" t="s">
@@ -12986,7 +13235,7 @@
       <c r="AA58" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AB58" s="168">
+      <c r="AB58" s="163">
         <v>8000</v>
       </c>
       <c r="AC58" s="2" t="s">
@@ -13013,7 +13262,7 @@
       <c r="AR58" s="35"/>
       <c r="AS58" s="35"/>
     </row>
-    <row r="59" spans="1:45" ht="16">
+    <row r="59" spans="1:45" ht="29">
       <c r="A59" s="7" t="s">
         <v>153</v>
       </c>
@@ -13091,7 +13340,7 @@
       <c r="AA59" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AB59" s="168">
+      <c r="AB59" s="163">
         <v>10688</v>
       </c>
       <c r="AC59" s="2" t="s">
@@ -13204,7 +13453,7 @@
       <c r="AR60" s="35"/>
       <c r="AS60" s="35"/>
     </row>
-    <row r="61" spans="1:45" ht="13">
+    <row r="61" spans="1:45" ht="70">
       <c r="A61" s="7" t="s">
         <v>1433</v>
       </c>
@@ -13292,7 +13541,7 @@
       <c r="AR61" s="35"/>
       <c r="AS61" s="35"/>
     </row>
-    <row r="62" spans="1:45" ht="16">
+    <row r="62" spans="1:45" ht="43">
       <c r="A62" s="7" t="s">
         <v>153</v>
       </c>
@@ -13462,7 +13711,7 @@
       <c r="AA63" s="2" t="s">
         <v>1540</v>
       </c>
-      <c r="AB63" s="169">
+      <c r="AB63" s="164">
         <v>64000</v>
       </c>
       <c r="AC63" s="2" t="s">
@@ -13565,7 +13814,7 @@
       <c r="AA64" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB64" s="168">
+      <c r="AB64" s="163">
         <v>1336</v>
       </c>
       <c r="AC64" s="7" t="s">
@@ -13668,7 +13917,7 @@
       <c r="AA65" s="2" t="s">
         <v>1518</v>
       </c>
-      <c r="AB65" s="168">
+      <c r="AB65" s="163">
         <v>32000</v>
       </c>
       <c r="AC65" s="7" t="s">
@@ -13953,7 +14202,7 @@
       <c r="AA68" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AB68" s="168">
+      <c r="AB68" s="163">
         <v>1670</v>
       </c>
       <c r="AC68" s="7" t="s">
@@ -14246,7 +14495,7 @@
       <c r="AR71" s="35"/>
       <c r="AS71" s="35"/>
     </row>
-    <row r="72" spans="1:45" ht="15">
+    <row r="72" spans="1:45" ht="29">
       <c r="A72" s="7" t="s">
         <v>153</v>
       </c>
@@ -14580,7 +14829,7 @@
       <c r="AA75" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AB75" s="168">
+      <c r="AB75" s="163">
         <v>2672</v>
       </c>
       <c r="AC75" s="7" t="s">
@@ -14607,7 +14856,7 @@
       <c r="AR75" s="35"/>
       <c r="AS75" s="35"/>
     </row>
-    <row r="76" spans="1:45" ht="13">
+    <row r="76" spans="1:45" ht="28">
       <c r="A76" s="7" t="s">
         <v>217</v>
       </c>
@@ -14691,7 +14940,7 @@
       <c r="AR76" s="35"/>
       <c r="AS76" s="35"/>
     </row>
-    <row r="77" spans="1:45" ht="13">
+    <row r="77" spans="1:45" ht="56">
       <c r="A77" s="7" t="s">
         <v>153</v>
       </c>
@@ -14861,7 +15110,7 @@
       <c r="AR78" s="35"/>
       <c r="AS78" s="35"/>
     </row>
-    <row r="79" spans="1:45" ht="13">
+    <row r="79" spans="1:45" ht="28">
       <c r="A79" s="7" t="s">
         <v>153</v>
       </c>
@@ -14951,7 +15200,7 @@
       <c r="AR79" s="35"/>
       <c r="AS79" s="35"/>
     </row>
-    <row r="80" spans="1:45" ht="13">
+    <row r="80" spans="1:45" ht="28">
       <c r="A80" s="7" t="s">
         <v>153</v>
       </c>
@@ -15123,7 +15372,7 @@
       <c r="AA81" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB81" s="168">
+      <c r="AB81" s="163">
         <v>395456</v>
       </c>
       <c r="AC81" s="7" t="s">
@@ -15220,7 +15469,7 @@
       <c r="AA82" s="2" t="s">
         <v>1518</v>
       </c>
-      <c r="AB82" s="168">
+      <c r="AB82" s="163">
         <v>334</v>
       </c>
       <c r="AC82" s="7" t="s">
@@ -15401,7 +15650,7 @@
       <c r="AA84" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AB84" s="168">
+      <c r="AB84" s="163">
         <v>3633</v>
       </c>
       <c r="AC84" s="7" t="s">
@@ -15500,7 +15749,7 @@
       <c r="AA85" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AB85" s="168">
+      <c r="AB85" s="163">
         <v>1336</v>
       </c>
       <c r="AC85" s="7" t="s">
@@ -15527,7 +15776,7 @@
       <c r="AR85" s="35"/>
       <c r="AS85" s="35"/>
     </row>
-    <row r="86" spans="1:45" ht="13">
+    <row r="86" spans="1:45" ht="70">
       <c r="A86" s="7" t="s">
         <v>1086</v>
       </c>
@@ -15613,7 +15862,7 @@
       <c r="AR86" s="35"/>
       <c r="AS86" s="35"/>
     </row>
-    <row r="87" spans="1:45" ht="13">
+    <row r="87" spans="1:45" ht="28">
       <c r="A87" s="7" t="s">
         <v>1433</v>
       </c>
@@ -15781,7 +16030,7 @@
       <c r="AA88" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AB88" s="168">
+      <c r="AB88" s="163">
         <v>4008</v>
       </c>
       <c r="AC88" s="2" t="s">
@@ -15894,7 +16143,7 @@
       <c r="AR89" s="35"/>
       <c r="AS89" s="35"/>
     </row>
-    <row r="90" spans="1:45" ht="13">
+    <row r="90" spans="1:45" ht="28">
       <c r="A90" s="7" t="s">
         <v>153</v>
       </c>
@@ -15962,7 +16211,7 @@
       <c r="AA90" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AB90" s="168">
+      <c r="AB90" s="163">
         <v>9683.5499999999993</v>
       </c>
       <c r="AC90" s="7" t="s">
@@ -16141,7 +16390,7 @@
       <c r="AA92" s="2" t="s">
         <v>1518</v>
       </c>
-      <c r="AB92" s="168">
+      <c r="AB92" s="163">
         <v>334</v>
       </c>
       <c r="AC92" s="2" t="s">
@@ -16242,7 +16491,7 @@
       <c r="AA93" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AB93" s="168">
+      <c r="AB93" s="163">
         <v>5344</v>
       </c>
       <c r="AC93" s="2" t="s">
@@ -16345,7 +16594,7 @@
       <c r="AA94" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB94" s="168">
+      <c r="AB94" s="163">
         <v>9352</v>
       </c>
       <c r="AC94" s="7" t="s">
@@ -16372,7 +16621,7 @@
       <c r="AR94" s="35"/>
       <c r="AS94" s="35"/>
     </row>
-    <row r="95" spans="1:45" ht="13">
+    <row r="95" spans="1:45" ht="28">
       <c r="A95" s="7" t="s">
         <v>153</v>
       </c>
@@ -16550,7 +16799,7 @@
       <c r="AR96" s="35"/>
       <c r="AS96" s="35"/>
     </row>
-    <row r="97" spans="1:45" ht="13">
+    <row r="97" spans="1:45" ht="56">
       <c r="A97" s="7" t="s">
         <v>153</v>
       </c>
@@ -16638,7 +16887,7 @@
       <c r="AR97" s="35"/>
       <c r="AS97" s="35"/>
     </row>
-    <row r="98" spans="1:45" ht="13">
+    <row r="98" spans="1:45" ht="84">
       <c r="A98" s="7" t="s">
         <v>1433</v>
       </c>
@@ -16996,7 +17245,7 @@
       <c r="AR101" s="35"/>
       <c r="AS101" s="35"/>
     </row>
-    <row r="102" spans="1:45" ht="13">
+    <row r="102" spans="1:45" ht="28">
       <c r="A102" s="7" t="s">
         <v>1433</v>
       </c>
@@ -17166,7 +17415,7 @@
       <c r="AR103" s="35"/>
       <c r="AS103" s="35"/>
     </row>
-    <row r="104" spans="1:45" ht="13">
+    <row r="104" spans="1:45" ht="28">
       <c r="A104" s="7" t="s">
         <v>153</v>
       </c>
@@ -17418,7 +17667,7 @@
         <v>170</v>
       </c>
       <c r="AA106" s="2"/>
-      <c r="AB106" s="168">
+      <c r="AB106" s="163">
         <v>1336</v>
       </c>
       <c r="AC106" s="148" t="s">
@@ -17515,7 +17764,7 @@
       <c r="AA107" s="2" t="s">
         <v>1518</v>
       </c>
-      <c r="AB107" s="168">
+      <c r="AB107" s="163">
         <v>119.48</v>
       </c>
       <c r="AC107" s="148" t="s">
@@ -17628,7 +17877,7 @@
       <c r="AR108" s="35"/>
       <c r="AS108" s="35"/>
     </row>
-    <row r="109" spans="1:45" ht="13">
+    <row r="109" spans="1:45" ht="42">
       <c r="A109" s="7" t="s">
         <v>1433</v>
       </c>
@@ -17722,7 +17971,7 @@
       <c r="AR109" s="35"/>
       <c r="AS109" s="35"/>
     </row>
-    <row r="110" spans="1:45" ht="16">
+    <row r="110" spans="1:45" ht="119">
       <c r="A110" s="7" t="s">
         <v>1086</v>
       </c>
@@ -17756,7 +18005,7 @@
       </c>
       <c r="N110" s="81"/>
       <c r="O110" s="40"/>
-      <c r="P110" s="167" t="s">
+      <c r="P110" s="162" t="s">
         <v>1857</v>
       </c>
       <c r="Q110" s="7" t="s">
@@ -17896,7 +18145,7 @@
       <c r="AR111" s="35"/>
       <c r="AS111" s="35"/>
     </row>
-    <row r="112" spans="1:45" ht="16">
+    <row r="112" spans="1:45" ht="29">
       <c r="A112" s="7" t="s">
         <v>619</v>
       </c>
@@ -18054,7 +18303,7 @@
       <c r="AA113" s="2" t="s">
         <v>1518</v>
       </c>
-      <c r="AB113" s="168">
+      <c r="AB113" s="163">
         <v>1688</v>
       </c>
       <c r="AC113" s="7" t="s">
@@ -18151,7 +18400,7 @@
       <c r="AA114" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB114" s="168">
+      <c r="AB114" s="163">
         <v>2672</v>
       </c>
       <c r="AC114" s="7" t="s">
@@ -18338,7 +18587,7 @@
       <c r="AA116" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AB116" s="168">
+      <c r="AB116" s="163">
         <v>334</v>
       </c>
       <c r="AC116" s="2" t="s">
@@ -18523,7 +18772,7 @@
       <c r="AA118" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AB118" s="168">
+      <c r="AB118" s="163">
         <v>1670</v>
       </c>
       <c r="AC118" s="7" t="s">
@@ -18606,7 +18855,7 @@
       <c r="AA119" s="107" t="s">
         <v>1897</v>
       </c>
-      <c r="AB119" s="168">
+      <c r="AB119" s="163">
         <v>8016</v>
       </c>
       <c r="AC119" s="100" t="s">
@@ -18707,7 +18956,7 @@
       <c r="AA120" s="2" t="s">
         <v>1794</v>
       </c>
-      <c r="AB120" s="168">
+      <c r="AB120" s="163">
         <v>1818.4</v>
       </c>
       <c r="AC120" s="2" t="s">
@@ -18734,7 +18983,7 @@
       <c r="AR120" s="35"/>
       <c r="AS120" s="35"/>
     </row>
-    <row r="121" spans="1:45" ht="13">
+    <row r="121" spans="1:45" ht="42">
       <c r="A121" s="7" t="s">
         <v>1433</v>
       </c>
@@ -18806,7 +19055,7 @@
       <c r="AA121" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AB121" s="168">
+      <c r="AB121" s="163">
         <v>1670</v>
       </c>
       <c r="AC121" s="2" t="s">
@@ -18987,7 +19236,7 @@
       <c r="AA123" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB123" s="168">
+      <c r="AB123" s="163">
         <v>142952</v>
       </c>
       <c r="AC123" s="2" t="s">
@@ -19190,7 +19439,7 @@
       <c r="AR125" s="35"/>
       <c r="AS125" s="35"/>
     </row>
-    <row r="126" spans="1:45" ht="13">
+    <row r="126" spans="1:45" ht="56">
       <c r="A126" s="7" t="s">
         <v>1433</v>
       </c>
@@ -19538,7 +19787,7 @@
       <c r="AA129" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB129" s="168">
+      <c r="AB129" s="163">
         <v>4186</v>
       </c>
       <c r="AC129" s="2" t="s">
@@ -19635,7 +19884,7 @@
       <c r="AA130" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB130" s="168">
+      <c r="AB130" s="163">
         <v>2182</v>
       </c>
       <c r="AC130" s="2" t="s">
@@ -19732,7 +19981,7 @@
       <c r="AA131" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB131" s="168">
+      <c r="AB131" s="163">
         <v>5229</v>
       </c>
       <c r="AC131" s="2" t="s">
@@ -19829,7 +20078,7 @@
       <c r="AA132" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB132" s="168">
+      <c r="AB132" s="163">
         <v>4141</v>
       </c>
       <c r="AC132" s="2" t="s">
@@ -20098,7 +20347,7 @@
       <c r="AA135" s="127" t="s">
         <v>50</v>
       </c>
-      <c r="AB135" s="168">
+      <c r="AB135" s="163">
         <v>243152</v>
       </c>
       <c r="AC135" s="120" t="s">
@@ -20371,7 +20620,7 @@
       <c r="AA138" s="127" t="s">
         <v>1976</v>
       </c>
-      <c r="AB138" s="168">
+      <c r="AB138" s="163">
         <v>534</v>
       </c>
       <c r="AC138" s="120" t="s">
@@ -20804,7 +21053,7 @@
       </c>
       <c r="Z143" s="40"/>
       <c r="AA143" s="35"/>
-      <c r="AB143" s="168">
+      <c r="AB143" s="163">
         <v>1332</v>
       </c>
       <c r="AC143" s="2" t="s">
@@ -20901,7 +21150,7 @@
       <c r="AA144" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AB144" s="168">
+      <c r="AB144" s="163">
         <v>5344</v>
       </c>
       <c r="AC144" s="7" t="s">
@@ -20988,7 +21237,7 @@
       <c r="AA145" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AB145" s="168">
+      <c r="AB145" s="163">
         <v>8350</v>
       </c>
       <c r="AC145" s="7" t="s">
@@ -21016,832 +21265,1682 @@
       <c r="AS145" s="35"/>
     </row>
     <row r="146" spans="1:45" ht="13">
-      <c r="A146" s="40"/>
-      <c r="B146" s="40"/>
-      <c r="C146" s="40"/>
-      <c r="D146" s="7"/>
-      <c r="E146" s="40"/>
-      <c r="F146" s="40"/>
-      <c r="G146" s="40"/>
-      <c r="H146" s="40"/>
-      <c r="I146" s="40"/>
-      <c r="J146" s="40"/>
-      <c r="K146" s="40"/>
-      <c r="L146" s="40"/>
-      <c r="M146" s="40"/>
-      <c r="N146" s="81"/>
-      <c r="O146" s="40"/>
-      <c r="P146" s="153"/>
-      <c r="Q146" s="40"/>
-      <c r="R146" s="3"/>
-      <c r="S146" s="40"/>
-      <c r="T146" s="20"/>
-      <c r="U146" s="7"/>
-      <c r="V146" s="40"/>
-      <c r="W146" s="40"/>
-      <c r="X146" s="40"/>
-      <c r="Y146" s="40"/>
-      <c r="Z146" s="40"/>
-      <c r="AA146" s="35"/>
-      <c r="AC146" s="35"/>
-      <c r="AD146" s="2"/>
-      <c r="AE146" s="35"/>
-      <c r="AF146" s="35"/>
-      <c r="AG146" s="35"/>
-      <c r="AH146" s="35"/>
-      <c r="AI146" s="35"/>
-      <c r="AJ146" s="35"/>
-      <c r="AK146" s="35"/>
-      <c r="AL146" s="35"/>
-      <c r="AM146" s="35"/>
-      <c r="AN146" s="35"/>
-      <c r="AO146" s="35"/>
-      <c r="AP146" s="35"/>
-      <c r="AQ146" s="35"/>
-      <c r="AR146" s="35"/>
-      <c r="AS146" s="35"/>
+      <c r="A146" s="154">
+        <v>2015</v>
+      </c>
+      <c r="B146" s="154">
+        <v>9</v>
+      </c>
+      <c r="C146" s="154">
+        <v>14</v>
+      </c>
+      <c r="D146" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E146" s="170" t="s">
+        <v>420</v>
+      </c>
+      <c r="F146" s="170" t="s">
+        <v>2021</v>
+      </c>
+      <c r="G146" s="170" t="s">
+        <v>45</v>
+      </c>
+      <c r="H146" s="170" t="s">
+        <v>2022</v>
+      </c>
+      <c r="I146" s="170" t="s">
+        <v>2023</v>
+      </c>
+      <c r="J146" s="170" t="s">
+        <v>2024</v>
+      </c>
+      <c r="K146" s="170"/>
+      <c r="L146" s="170" t="s">
+        <v>2025</v>
+      </c>
+      <c r="M146" s="170"/>
+      <c r="N146" s="171">
+        <v>3572464</v>
+      </c>
+      <c r="O146" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="P146" s="170" t="s">
+        <v>2026</v>
+      </c>
+      <c r="Q146" s="170"/>
+      <c r="R146" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S146" s="170">
+        <v>4</v>
+      </c>
+      <c r="T146" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U146" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V146" s="172" t="s">
+        <v>2027</v>
+      </c>
+      <c r="W146" s="170"/>
+      <c r="X146" s="170" t="s">
+        <v>412</v>
+      </c>
+      <c r="Y146" s="170"/>
+      <c r="Z146" s="170">
+        <v>2674</v>
+      </c>
+      <c r="AA146" s="170" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB146" s="171">
+        <v>3572464</v>
+      </c>
+      <c r="AC146" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD146" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE146" s="170"/>
+      <c r="AF146" s="170"/>
+      <c r="AG146" s="170"/>
+      <c r="AH146" s="170"/>
+      <c r="AI146" s="170"/>
+      <c r="AJ146" s="170"/>
+      <c r="AK146" s="170"/>
+      <c r="AL146" s="170"/>
+      <c r="AM146" s="170"/>
+      <c r="AN146" s="170"/>
+      <c r="AO146" s="170"/>
+      <c r="AP146" s="170"/>
+      <c r="AQ146" s="170"/>
+      <c r="AR146" s="170"/>
+      <c r="AS146" s="170"/>
     </row>
     <row r="147" spans="1:45" ht="13">
-      <c r="A147" s="40"/>
-      <c r="B147" s="40"/>
-      <c r="C147" s="40"/>
-      <c r="D147" s="7"/>
-      <c r="E147" s="40"/>
-      <c r="F147" s="40"/>
-      <c r="G147" s="40"/>
-      <c r="H147" s="40"/>
-      <c r="I147" s="40"/>
-      <c r="J147" s="40"/>
-      <c r="K147" s="40"/>
-      <c r="L147" s="40"/>
-      <c r="M147" s="40"/>
-      <c r="N147" s="81"/>
-      <c r="O147" s="40"/>
-      <c r="P147" s="153"/>
-      <c r="Q147" s="40"/>
-      <c r="R147" s="3"/>
-      <c r="S147" s="40"/>
-      <c r="T147" s="20"/>
-      <c r="U147" s="7"/>
-      <c r="V147" s="40"/>
-      <c r="W147" s="40"/>
-      <c r="X147" s="40"/>
-      <c r="Y147" s="40"/>
-      <c r="Z147" s="40"/>
-      <c r="AA147" s="35"/>
-      <c r="AC147" s="35"/>
-      <c r="AD147" s="2"/>
-      <c r="AE147" s="35"/>
-      <c r="AF147" s="35"/>
-      <c r="AG147" s="35"/>
-      <c r="AH147" s="35"/>
-      <c r="AI147" s="35"/>
-      <c r="AJ147" s="35"/>
-      <c r="AK147" s="35"/>
-      <c r="AL147" s="35"/>
-      <c r="AM147" s="35"/>
-      <c r="AN147" s="35"/>
-      <c r="AO147" s="35"/>
-      <c r="AP147" s="35"/>
-      <c r="AQ147" s="35"/>
-      <c r="AR147" s="35"/>
-      <c r="AS147" s="35"/>
+      <c r="A147" s="154">
+        <v>2018</v>
+      </c>
+      <c r="B147" s="154">
+        <v>7</v>
+      </c>
+      <c r="C147" s="154">
+        <v>24</v>
+      </c>
+      <c r="D147" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E147" s="170" t="s">
+        <v>428</v>
+      </c>
+      <c r="F147" s="170" t="s">
+        <v>2028</v>
+      </c>
+      <c r="G147" s="170" t="s">
+        <v>45</v>
+      </c>
+      <c r="H147" s="170" t="s">
+        <v>2029</v>
+      </c>
+      <c r="I147" s="170"/>
+      <c r="J147" s="170" t="s">
+        <v>2030</v>
+      </c>
+      <c r="K147" s="170"/>
+      <c r="L147" s="170" t="s">
+        <v>1679</v>
+      </c>
+      <c r="M147" s="170"/>
+      <c r="N147" s="170"/>
+      <c r="O147" s="170"/>
+      <c r="P147" s="170" t="s">
+        <v>2031</v>
+      </c>
+      <c r="Q147" s="170"/>
+      <c r="R147" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S147" s="170">
+        <v>1</v>
+      </c>
+      <c r="T147" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U147" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V147" s="172" t="s">
+        <v>2032</v>
+      </c>
+      <c r="W147" s="170"/>
+      <c r="X147" s="170" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y147" s="170" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z147" s="170">
+        <v>497.3</v>
+      </c>
+      <c r="AA147" s="170" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB147" s="170"/>
+      <c r="AC147" s="170"/>
+      <c r="AD147" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE147" s="170"/>
+      <c r="AF147" s="170" t="s">
+        <v>2033</v>
+      </c>
+      <c r="AG147" s="170"/>
+      <c r="AH147" s="170"/>
+      <c r="AI147" s="170"/>
+      <c r="AJ147" s="170"/>
+      <c r="AK147" s="170"/>
+      <c r="AL147" s="170"/>
+      <c r="AM147" s="170"/>
+      <c r="AN147" s="170"/>
+      <c r="AO147" s="170"/>
+      <c r="AP147" s="170"/>
+      <c r="AQ147" s="170"/>
+      <c r="AR147" s="170"/>
+      <c r="AS147" s="170"/>
     </row>
     <row r="148" spans="1:45" ht="13">
-      <c r="A148" s="40"/>
-      <c r="B148" s="40"/>
-      <c r="C148" s="40"/>
-      <c r="D148" s="7"/>
-      <c r="E148" s="40"/>
-      <c r="F148" s="40"/>
-      <c r="G148" s="40"/>
-      <c r="H148" s="40"/>
-      <c r="I148" s="40"/>
-      <c r="J148" s="40"/>
-      <c r="K148" s="40"/>
-      <c r="L148" s="40"/>
-      <c r="M148" s="40"/>
-      <c r="N148" s="81"/>
-      <c r="O148" s="40"/>
-      <c r="P148" s="153"/>
-      <c r="Q148" s="40"/>
-      <c r="R148" s="3"/>
-      <c r="S148" s="40"/>
-      <c r="T148" s="20"/>
-      <c r="U148" s="7"/>
-      <c r="V148" s="40"/>
-      <c r="W148" s="40"/>
-      <c r="X148" s="40"/>
-      <c r="Y148" s="40"/>
-      <c r="Z148" s="40"/>
-      <c r="AA148" s="35"/>
-      <c r="AC148" s="35"/>
-      <c r="AD148" s="2"/>
-      <c r="AE148" s="35"/>
-      <c r="AF148" s="35"/>
-      <c r="AG148" s="35"/>
-      <c r="AH148" s="35"/>
-      <c r="AI148" s="35"/>
-      <c r="AJ148" s="35"/>
-      <c r="AK148" s="35"/>
-      <c r="AL148" s="35"/>
-      <c r="AM148" s="35"/>
-      <c r="AN148" s="35"/>
-      <c r="AO148" s="35"/>
-      <c r="AP148" s="35"/>
-      <c r="AQ148" s="35"/>
-      <c r="AR148" s="35"/>
-      <c r="AS148" s="35"/>
-    </row>
-    <row r="149" spans="1:45" ht="13">
-      <c r="A149" s="40"/>
-      <c r="B149" s="40"/>
-      <c r="C149" s="40"/>
-      <c r="D149" s="7"/>
-      <c r="E149" s="40"/>
-      <c r="F149" s="40"/>
-      <c r="G149" s="40"/>
-      <c r="H149" s="40"/>
-      <c r="I149" s="40"/>
-      <c r="J149" s="40"/>
-      <c r="K149" s="40"/>
-      <c r="L149" s="40"/>
-      <c r="M149" s="40"/>
-      <c r="N149" s="81"/>
-      <c r="O149" s="40"/>
-      <c r="P149" s="153"/>
-      <c r="Q149" s="40"/>
-      <c r="R149" s="3"/>
-      <c r="S149" s="40"/>
-      <c r="T149" s="20"/>
-      <c r="U149" s="7"/>
-      <c r="V149" s="40"/>
-      <c r="W149" s="40"/>
-      <c r="X149" s="40"/>
-      <c r="Y149" s="40"/>
-      <c r="Z149" s="40"/>
-      <c r="AA149" s="35"/>
-      <c r="AC149" s="35"/>
-      <c r="AD149" s="2"/>
-      <c r="AE149" s="35"/>
-      <c r="AF149" s="35"/>
-      <c r="AG149" s="35"/>
-      <c r="AH149" s="35"/>
-      <c r="AI149" s="35"/>
-      <c r="AJ149" s="35"/>
-      <c r="AK149" s="35"/>
-      <c r="AL149" s="35"/>
-      <c r="AM149" s="35"/>
-      <c r="AN149" s="35"/>
-      <c r="AO149" s="35"/>
-      <c r="AP149" s="35"/>
-      <c r="AQ149" s="35"/>
-      <c r="AR149" s="35"/>
-      <c r="AS149" s="35"/>
+      <c r="A148" s="154">
+        <v>2016</v>
+      </c>
+      <c r="B148" s="154">
+        <v>4</v>
+      </c>
+      <c r="C148" s="154">
+        <v>11</v>
+      </c>
+      <c r="D148" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E148" s="170" t="s">
+        <v>420</v>
+      </c>
+      <c r="F148" s="170" t="s">
+        <v>2034</v>
+      </c>
+      <c r="G148" s="170" t="s">
+        <v>1980</v>
+      </c>
+      <c r="H148" s="170" t="s">
+        <v>2035</v>
+      </c>
+      <c r="I148" s="170"/>
+      <c r="J148" s="170" t="s">
+        <v>2036</v>
+      </c>
+      <c r="K148" s="170"/>
+      <c r="L148" s="170" t="s">
+        <v>2037</v>
+      </c>
+      <c r="M148" s="170"/>
+      <c r="N148" s="171">
+        <v>1997320</v>
+      </c>
+      <c r="O148" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="P148" s="170" t="s">
+        <v>2038</v>
+      </c>
+      <c r="Q148" s="170"/>
+      <c r="R148" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S148" s="170">
+        <v>1</v>
+      </c>
+      <c r="T148" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U148" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V148" s="172" t="s">
+        <v>2039</v>
+      </c>
+      <c r="W148" s="170"/>
+      <c r="X148" s="170" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y148" s="170" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z148" s="170">
+        <v>1495</v>
+      </c>
+      <c r="AA148" s="170" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB148" s="171">
+        <v>1997320</v>
+      </c>
+      <c r="AC148" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD148" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE148" s="170"/>
+      <c r="AF148" s="170"/>
+      <c r="AG148" s="170"/>
+      <c r="AH148" s="170"/>
+      <c r="AI148" s="170"/>
+      <c r="AJ148" s="170"/>
+      <c r="AK148" s="170"/>
+      <c r="AL148" s="170"/>
+      <c r="AM148" s="170"/>
+      <c r="AN148" s="170"/>
+      <c r="AO148" s="170"/>
+      <c r="AP148" s="170"/>
+      <c r="AQ148" s="170"/>
+      <c r="AR148" s="170"/>
+      <c r="AS148" s="170"/>
+    </row>
+    <row r="149" spans="1:45" ht="28">
+      <c r="A149" s="154">
+        <v>2016</v>
+      </c>
+      <c r="B149" s="154">
+        <v>10</v>
+      </c>
+      <c r="C149" s="154">
+        <v>9</v>
+      </c>
+      <c r="D149" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E149" s="170" t="s">
+        <v>428</v>
+      </c>
+      <c r="F149" s="170" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G149" s="173" t="s">
+        <v>1491</v>
+      </c>
+      <c r="H149" s="170" t="s">
+        <v>2040</v>
+      </c>
+      <c r="I149" s="170"/>
+      <c r="J149" s="170" t="s">
+        <v>2041</v>
+      </c>
+      <c r="K149" s="170"/>
+      <c r="L149" s="170" t="s">
+        <v>1679</v>
+      </c>
+      <c r="M149" s="170"/>
+      <c r="N149" s="171">
+        <v>37408</v>
+      </c>
+      <c r="O149" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="P149" s="170" t="s">
+        <v>2042</v>
+      </c>
+      <c r="Q149" s="170"/>
+      <c r="R149" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S149" s="170">
+        <v>1</v>
+      </c>
+      <c r="T149" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U149" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V149" s="172" t="s">
+        <v>2043</v>
+      </c>
+      <c r="W149" s="170" t="s">
+        <v>179</v>
+      </c>
+      <c r="X149" s="170" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y149" s="170" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z149" s="170">
+        <v>10</v>
+      </c>
+      <c r="AA149" s="170" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB149" s="171">
+        <v>37408</v>
+      </c>
+      <c r="AC149" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD149" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE149" s="170"/>
+      <c r="AF149" s="170"/>
+      <c r="AG149" s="170"/>
+      <c r="AH149" s="170"/>
+      <c r="AI149" s="170"/>
+      <c r="AJ149" s="170"/>
+      <c r="AK149" s="170"/>
+      <c r="AL149" s="170"/>
+      <c r="AM149" s="170"/>
+      <c r="AN149" s="170"/>
+      <c r="AO149" s="170"/>
+      <c r="AP149" s="170"/>
+      <c r="AQ149" s="170"/>
+      <c r="AR149" s="170"/>
+      <c r="AS149" s="170"/>
     </row>
     <row r="150" spans="1:45" ht="13">
-      <c r="A150" s="40"/>
-      <c r="B150" s="40"/>
-      <c r="C150" s="40"/>
-      <c r="D150" s="7"/>
-      <c r="E150" s="40"/>
-      <c r="F150" s="40"/>
-      <c r="G150" s="40"/>
-      <c r="H150" s="40"/>
-      <c r="I150" s="40"/>
-      <c r="J150" s="40"/>
-      <c r="K150" s="40"/>
-      <c r="L150" s="40"/>
-      <c r="M150" s="40"/>
-      <c r="N150" s="81"/>
-      <c r="O150" s="40"/>
-      <c r="P150" s="153"/>
-      <c r="Q150" s="40"/>
-      <c r="R150" s="3"/>
-      <c r="S150" s="40"/>
-      <c r="T150" s="20"/>
-      <c r="U150" s="7"/>
-      <c r="V150" s="40"/>
-      <c r="W150" s="40"/>
-      <c r="X150" s="40"/>
-      <c r="Y150" s="40"/>
-      <c r="Z150" s="40"/>
-      <c r="AA150" s="35"/>
-      <c r="AC150" s="35"/>
-      <c r="AD150" s="2"/>
-      <c r="AE150" s="35"/>
-      <c r="AF150" s="35"/>
-      <c r="AG150" s="35"/>
-      <c r="AH150" s="35"/>
-      <c r="AI150" s="35"/>
-      <c r="AJ150" s="35"/>
-      <c r="AK150" s="35"/>
-      <c r="AL150" s="35"/>
-      <c r="AM150" s="35"/>
-      <c r="AN150" s="35"/>
-      <c r="AO150" s="35"/>
-      <c r="AP150" s="35"/>
-      <c r="AQ150" s="35"/>
-      <c r="AR150" s="35"/>
-      <c r="AS150" s="35"/>
+      <c r="A150" s="154">
+        <v>2017</v>
+      </c>
+      <c r="B150" s="154">
+        <v>1</v>
+      </c>
+      <c r="C150" s="154">
+        <v>5</v>
+      </c>
+      <c r="D150" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E150" s="170" t="s">
+        <v>428</v>
+      </c>
+      <c r="F150" s="170" t="s">
+        <v>1504</v>
+      </c>
+      <c r="G150" s="170" t="s">
+        <v>407</v>
+      </c>
+      <c r="H150" s="170" t="s">
+        <v>2044</v>
+      </c>
+      <c r="I150" s="170"/>
+      <c r="J150" s="170" t="s">
+        <v>2045</v>
+      </c>
+      <c r="K150" s="170"/>
+      <c r="L150" s="170" t="s">
+        <v>2046</v>
+      </c>
+      <c r="M150" s="170"/>
+      <c r="N150" s="171">
+        <v>1152001</v>
+      </c>
+      <c r="O150" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="P150" s="170" t="s">
+        <v>2047</v>
+      </c>
+      <c r="Q150" s="170"/>
+      <c r="R150" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S150" s="170">
+        <v>3</v>
+      </c>
+      <c r="T150" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U150" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V150" s="172" t="s">
+        <v>2048</v>
+      </c>
+      <c r="W150" s="170"/>
+      <c r="X150" s="170" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y150" s="170" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z150" s="170">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="AA150" s="170" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB150" s="171">
+        <v>2247</v>
+      </c>
+      <c r="AC150" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD150" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE150" s="170"/>
+      <c r="AF150" s="170" t="s">
+        <v>2049</v>
+      </c>
+      <c r="AG150" s="170"/>
+      <c r="AH150" s="170"/>
+      <c r="AI150" s="170"/>
+      <c r="AJ150" s="170"/>
+      <c r="AK150" s="170"/>
+      <c r="AL150" s="170"/>
+      <c r="AM150" s="170"/>
+      <c r="AN150" s="170"/>
+      <c r="AO150" s="170"/>
+      <c r="AP150" s="170"/>
+      <c r="AQ150" s="170"/>
+      <c r="AR150" s="170"/>
+      <c r="AS150" s="170"/>
     </row>
     <row r="151" spans="1:45" ht="13">
-      <c r="A151" s="40"/>
-      <c r="B151" s="40"/>
-      <c r="C151" s="40"/>
-      <c r="D151" s="7"/>
-      <c r="E151" s="40"/>
-      <c r="F151" s="40"/>
-      <c r="G151" s="40"/>
-      <c r="H151" s="40"/>
-      <c r="I151" s="40"/>
-      <c r="J151" s="40"/>
-      <c r="K151" s="40"/>
-      <c r="L151" s="40"/>
-      <c r="M151" s="40"/>
-      <c r="N151" s="81"/>
-      <c r="O151" s="40"/>
-      <c r="P151" s="153"/>
-      <c r="Q151" s="40"/>
-      <c r="R151" s="3"/>
-      <c r="S151" s="40"/>
-      <c r="T151" s="20"/>
-      <c r="U151" s="7"/>
-      <c r="V151" s="40"/>
-      <c r="W151" s="40"/>
-      <c r="X151" s="40"/>
-      <c r="Y151" s="40"/>
-      <c r="Z151" s="40"/>
-      <c r="AA151" s="35"/>
-      <c r="AC151" s="35"/>
-      <c r="AD151" s="2"/>
-      <c r="AE151" s="35"/>
-      <c r="AF151" s="35"/>
-      <c r="AG151" s="35"/>
-      <c r="AH151" s="35"/>
-      <c r="AI151" s="35"/>
-      <c r="AJ151" s="35"/>
-      <c r="AK151" s="35"/>
-      <c r="AL151" s="35"/>
-      <c r="AM151" s="35"/>
-      <c r="AN151" s="35"/>
-      <c r="AO151" s="35"/>
-      <c r="AP151" s="35"/>
-      <c r="AQ151" s="35"/>
-      <c r="AR151" s="35"/>
-      <c r="AS151" s="35"/>
+      <c r="A151" s="154">
+        <v>2018</v>
+      </c>
+      <c r="B151" s="154">
+        <v>2</v>
+      </c>
+      <c r="C151" s="154">
+        <v>24</v>
+      </c>
+      <c r="D151" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E151" s="170" t="s">
+        <v>428</v>
+      </c>
+      <c r="F151" s="170" t="s">
+        <v>1462</v>
+      </c>
+      <c r="G151" s="170" t="s">
+        <v>407</v>
+      </c>
+      <c r="H151" s="170"/>
+      <c r="I151" s="170"/>
+      <c r="J151" s="170"/>
+      <c r="K151" s="170"/>
+      <c r="L151" s="170"/>
+      <c r="M151" s="170"/>
+      <c r="N151" s="170">
+        <v>2241</v>
+      </c>
+      <c r="O151" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="P151" s="170" t="s">
+        <v>2050</v>
+      </c>
+      <c r="Q151" s="170"/>
+      <c r="R151" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S151" s="170">
+        <v>1</v>
+      </c>
+      <c r="T151" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U151" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V151" s="172" t="s">
+        <v>2051</v>
+      </c>
+      <c r="W151" s="170"/>
+      <c r="X151" s="170" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y151" s="170" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z151" s="170">
+        <v>31.7</v>
+      </c>
+      <c r="AA151" s="170" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB151" s="170"/>
+      <c r="AC151" s="170"/>
+      <c r="AD151" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE151" s="170"/>
+      <c r="AF151" s="170" t="s">
+        <v>2052</v>
+      </c>
+      <c r="AG151" s="170"/>
+      <c r="AH151" s="170"/>
+      <c r="AI151" s="170"/>
+      <c r="AJ151" s="170"/>
+      <c r="AK151" s="170"/>
+      <c r="AL151" s="170"/>
+      <c r="AM151" s="170"/>
+      <c r="AN151" s="170"/>
+      <c r="AO151" s="170"/>
+      <c r="AP151" s="170"/>
+      <c r="AQ151" s="170"/>
+      <c r="AR151" s="170"/>
+      <c r="AS151" s="170"/>
     </row>
     <row r="152" spans="1:45" ht="13">
-      <c r="A152" s="40"/>
-      <c r="B152" s="40"/>
-      <c r="C152" s="40"/>
-      <c r="D152" s="7"/>
-      <c r="E152" s="40"/>
-      <c r="F152" s="40"/>
-      <c r="G152" s="40"/>
-      <c r="H152" s="40"/>
-      <c r="I152" s="40"/>
-      <c r="J152" s="40"/>
-      <c r="K152" s="40"/>
-      <c r="L152" s="40"/>
-      <c r="M152" s="40"/>
-      <c r="N152" s="81"/>
-      <c r="O152" s="40"/>
-      <c r="P152" s="153"/>
-      <c r="Q152" s="40"/>
-      <c r="R152" s="3"/>
-      <c r="S152" s="40"/>
-      <c r="T152" s="20"/>
-      <c r="U152" s="7"/>
-      <c r="V152" s="40"/>
-      <c r="W152" s="40"/>
-      <c r="X152" s="40"/>
-      <c r="Y152" s="40"/>
-      <c r="Z152" s="40"/>
-      <c r="AA152" s="35"/>
-      <c r="AC152" s="35"/>
-      <c r="AD152" s="2"/>
-      <c r="AE152" s="35"/>
-      <c r="AF152" s="35"/>
-      <c r="AG152" s="35"/>
-      <c r="AH152" s="35"/>
-      <c r="AI152" s="35"/>
-      <c r="AJ152" s="35"/>
-      <c r="AK152" s="35"/>
-      <c r="AL152" s="35"/>
-      <c r="AM152" s="35"/>
-      <c r="AN152" s="35"/>
-      <c r="AO152" s="35"/>
-      <c r="AP152" s="35"/>
-      <c r="AQ152" s="35"/>
-      <c r="AR152" s="35"/>
-      <c r="AS152" s="35"/>
+      <c r="A152" s="154">
+        <v>2016</v>
+      </c>
+      <c r="B152" s="154">
+        <v>12</v>
+      </c>
+      <c r="C152" s="154">
+        <v>9</v>
+      </c>
+      <c r="D152" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E152" s="170" t="s">
+        <v>1715</v>
+      </c>
+      <c r="F152" s="170"/>
+      <c r="G152" s="170" t="s">
+        <v>45</v>
+      </c>
+      <c r="H152" s="170" t="s">
+        <v>47</v>
+      </c>
+      <c r="I152" s="170"/>
+      <c r="J152" s="170" t="s">
+        <v>2053</v>
+      </c>
+      <c r="K152" s="170"/>
+      <c r="L152" s="170" t="s">
+        <v>2054</v>
+      </c>
+      <c r="M152" s="170"/>
+      <c r="N152" s="171">
+        <v>8309920</v>
+      </c>
+      <c r="O152" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="P152" s="170" t="s">
+        <v>2055</v>
+      </c>
+      <c r="Q152" s="170"/>
+      <c r="R152" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S152" s="170">
+        <v>2</v>
+      </c>
+      <c r="T152" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U152" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V152" s="172" t="s">
+        <v>2056</v>
+      </c>
+      <c r="W152" s="170"/>
+      <c r="X152" s="170" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y152" s="170" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z152" s="174">
+        <v>3110.05</v>
+      </c>
+      <c r="AA152" s="170" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB152" s="171">
+        <v>8309920</v>
+      </c>
+      <c r="AC152" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD152" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE152" s="170"/>
+      <c r="AF152" s="170"/>
+      <c r="AG152" s="170"/>
+      <c r="AH152" s="170"/>
+      <c r="AI152" s="170"/>
+      <c r="AJ152" s="170"/>
+      <c r="AK152" s="170"/>
+      <c r="AL152" s="170"/>
+      <c r="AM152" s="170"/>
+      <c r="AN152" s="170"/>
+      <c r="AO152" s="170"/>
+      <c r="AP152" s="170"/>
+      <c r="AQ152" s="170"/>
+      <c r="AR152" s="170"/>
+      <c r="AS152" s="170"/>
     </row>
     <row r="153" spans="1:45" ht="13">
-      <c r="A153" s="40"/>
-      <c r="B153" s="40"/>
-      <c r="C153" s="40"/>
-      <c r="D153" s="7"/>
-      <c r="E153" s="40"/>
-      <c r="F153" s="40"/>
-      <c r="G153" s="40"/>
-      <c r="H153" s="40"/>
-      <c r="I153" s="40"/>
-      <c r="J153" s="40"/>
-      <c r="K153" s="40"/>
-      <c r="L153" s="40"/>
-      <c r="M153" s="40"/>
-      <c r="N153" s="81"/>
-      <c r="O153" s="40"/>
-      <c r="P153" s="153"/>
-      <c r="Q153" s="40"/>
-      <c r="R153" s="3"/>
-      <c r="S153" s="40"/>
-      <c r="T153" s="20"/>
-      <c r="U153" s="7"/>
-      <c r="V153" s="40"/>
-      <c r="W153" s="40"/>
-      <c r="X153" s="40"/>
-      <c r="Y153" s="40"/>
-      <c r="Z153" s="40"/>
-      <c r="AA153" s="35"/>
-      <c r="AC153" s="35"/>
-      <c r="AD153" s="2"/>
-      <c r="AE153" s="35"/>
-      <c r="AF153" s="35"/>
-      <c r="AG153" s="35"/>
-      <c r="AH153" s="35"/>
-      <c r="AI153" s="35"/>
-      <c r="AJ153" s="35"/>
-      <c r="AK153" s="35"/>
-      <c r="AL153" s="35"/>
-      <c r="AM153" s="35"/>
-      <c r="AN153" s="35"/>
-      <c r="AO153" s="35"/>
-      <c r="AP153" s="35"/>
-      <c r="AQ153" s="35"/>
-      <c r="AR153" s="35"/>
-      <c r="AS153" s="35"/>
+      <c r="A153" s="154">
+        <v>2014</v>
+      </c>
+      <c r="B153" s="154">
+        <v>4</v>
+      </c>
+      <c r="C153" s="154">
+        <v>11</v>
+      </c>
+      <c r="D153" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E153" s="170" t="s">
+        <v>451</v>
+      </c>
+      <c r="F153" s="170" t="s">
+        <v>2057</v>
+      </c>
+      <c r="G153" s="170" t="s">
+        <v>45</v>
+      </c>
+      <c r="H153" s="170" t="s">
+        <v>1617</v>
+      </c>
+      <c r="I153" s="170" t="s">
+        <v>418</v>
+      </c>
+      <c r="J153" s="170" t="s">
+        <v>2058</v>
+      </c>
+      <c r="K153" s="170"/>
+      <c r="L153" s="170" t="s">
+        <v>1662</v>
+      </c>
+      <c r="M153" s="170"/>
+      <c r="N153" s="170"/>
+      <c r="O153" s="170"/>
+      <c r="P153" s="170"/>
+      <c r="Q153" s="170"/>
+      <c r="R153" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S153" s="170">
+        <v>1</v>
+      </c>
+      <c r="T153" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U153" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V153" s="172" t="s">
+        <v>2059</v>
+      </c>
+      <c r="W153" s="170"/>
+      <c r="X153" s="170" t="s">
+        <v>260</v>
+      </c>
+      <c r="Y153" s="170"/>
+      <c r="Z153" s="170">
+        <v>24</v>
+      </c>
+      <c r="AA153" s="170" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB153" s="170"/>
+      <c r="AC153" s="170"/>
+      <c r="AD153" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE153" s="170"/>
+      <c r="AF153" s="170" t="s">
+        <v>2060</v>
+      </c>
+      <c r="AG153" s="170"/>
+      <c r="AH153" s="170"/>
+      <c r="AI153" s="170"/>
+      <c r="AJ153" s="170"/>
+      <c r="AK153" s="170"/>
+      <c r="AL153" s="170"/>
+      <c r="AM153" s="170"/>
+      <c r="AN153" s="170"/>
+      <c r="AO153" s="170"/>
+      <c r="AP153" s="170"/>
+      <c r="AQ153" s="170"/>
+      <c r="AR153" s="170"/>
+      <c r="AS153" s="170"/>
     </row>
     <row r="154" spans="1:45" ht="13">
-      <c r="A154" s="40"/>
-      <c r="B154" s="40"/>
-      <c r="C154" s="40"/>
-      <c r="D154" s="7"/>
-      <c r="E154" s="40"/>
-      <c r="F154" s="40"/>
-      <c r="G154" s="40"/>
-      <c r="H154" s="40"/>
-      <c r="I154" s="40"/>
-      <c r="J154" s="40"/>
-      <c r="K154" s="40"/>
-      <c r="L154" s="40"/>
-      <c r="M154" s="40"/>
-      <c r="N154" s="81"/>
-      <c r="O154" s="40"/>
-      <c r="P154" s="153"/>
-      <c r="Q154" s="40"/>
-      <c r="R154" s="3"/>
-      <c r="S154" s="40"/>
-      <c r="T154" s="20"/>
-      <c r="U154" s="7"/>
-      <c r="V154" s="40"/>
-      <c r="W154" s="40"/>
-      <c r="X154" s="40"/>
-      <c r="Y154" s="40"/>
-      <c r="Z154" s="40"/>
-      <c r="AA154" s="35"/>
-      <c r="AC154" s="35"/>
-      <c r="AD154" s="2"/>
-      <c r="AE154" s="35"/>
-      <c r="AF154" s="35"/>
-      <c r="AG154" s="35"/>
-      <c r="AH154" s="35"/>
-      <c r="AI154" s="35"/>
-      <c r="AJ154" s="35"/>
-      <c r="AK154" s="35"/>
-      <c r="AL154" s="35"/>
-      <c r="AM154" s="35"/>
-      <c r="AN154" s="35"/>
-      <c r="AO154" s="35"/>
-      <c r="AP154" s="35"/>
-      <c r="AQ154" s="35"/>
-      <c r="AR154" s="35"/>
-      <c r="AS154" s="35"/>
-    </row>
-    <row r="155" spans="1:45" ht="13">
-      <c r="A155" s="40"/>
-      <c r="B155" s="40"/>
-      <c r="C155" s="40"/>
-      <c r="D155" s="7"/>
-      <c r="E155" s="40"/>
-      <c r="F155" s="40"/>
-      <c r="G155" s="40"/>
-      <c r="H155" s="40"/>
-      <c r="I155" s="40"/>
-      <c r="J155" s="40"/>
-      <c r="K155" s="40"/>
-      <c r="L155" s="40"/>
-      <c r="M155" s="40"/>
-      <c r="N155" s="81"/>
-      <c r="O155" s="40"/>
-      <c r="P155" s="153"/>
-      <c r="Q155" s="40"/>
-      <c r="R155" s="3"/>
-      <c r="S155" s="40"/>
-      <c r="T155" s="20"/>
-      <c r="U155" s="7"/>
-      <c r="V155" s="40"/>
-      <c r="W155" s="40"/>
-      <c r="X155" s="40"/>
-      <c r="Y155" s="40"/>
-      <c r="Z155" s="40"/>
-      <c r="AA155" s="35"/>
-      <c r="AC155" s="35"/>
-      <c r="AD155" s="2"/>
-      <c r="AE155" s="35"/>
-      <c r="AF155" s="35"/>
-      <c r="AG155" s="35"/>
-      <c r="AH155" s="35"/>
-      <c r="AI155" s="35"/>
-      <c r="AJ155" s="35"/>
-      <c r="AK155" s="35"/>
-      <c r="AL155" s="35"/>
-      <c r="AM155" s="35"/>
-      <c r="AN155" s="35"/>
-      <c r="AO155" s="35"/>
-      <c r="AP155" s="35"/>
-      <c r="AQ155" s="35"/>
-      <c r="AR155" s="35"/>
-      <c r="AS155" s="35"/>
-    </row>
-    <row r="156" spans="1:45" ht="13">
-      <c r="A156" s="40"/>
-      <c r="B156" s="40"/>
-      <c r="C156" s="40"/>
-      <c r="D156" s="7"/>
-      <c r="E156" s="40"/>
-      <c r="F156" s="40"/>
-      <c r="G156" s="40"/>
-      <c r="H156" s="40"/>
-      <c r="I156" s="40"/>
-      <c r="J156" s="40"/>
-      <c r="K156" s="40"/>
-      <c r="L156" s="40"/>
-      <c r="M156" s="40"/>
-      <c r="N156" s="81"/>
-      <c r="O156" s="40"/>
-      <c r="P156" s="153"/>
-      <c r="Q156" s="40"/>
-      <c r="R156" s="3"/>
-      <c r="S156" s="40"/>
-      <c r="T156" s="20"/>
-      <c r="U156" s="7"/>
-      <c r="V156" s="40"/>
-      <c r="W156" s="40"/>
-      <c r="X156" s="40"/>
-      <c r="Y156" s="40"/>
-      <c r="Z156" s="40"/>
-      <c r="AA156" s="35"/>
-      <c r="AC156" s="35"/>
-      <c r="AD156" s="2"/>
-      <c r="AE156" s="35"/>
-      <c r="AF156" s="35"/>
-      <c r="AG156" s="35"/>
-      <c r="AH156" s="35"/>
-      <c r="AI156" s="35"/>
-      <c r="AJ156" s="35"/>
-      <c r="AK156" s="35"/>
-      <c r="AL156" s="35"/>
-      <c r="AM156" s="35"/>
-      <c r="AN156" s="35"/>
-      <c r="AO156" s="35"/>
-      <c r="AP156" s="35"/>
-      <c r="AQ156" s="35"/>
-      <c r="AR156" s="35"/>
-      <c r="AS156" s="35"/>
-    </row>
-    <row r="157" spans="1:45" ht="13">
-      <c r="A157" s="40"/>
-      <c r="B157" s="40"/>
-      <c r="C157" s="40"/>
-      <c r="D157" s="7"/>
-      <c r="E157" s="40"/>
-      <c r="F157" s="40"/>
-      <c r="G157" s="40"/>
-      <c r="H157" s="40"/>
-      <c r="I157" s="40"/>
-      <c r="J157" s="40"/>
-      <c r="K157" s="40"/>
-      <c r="L157" s="40"/>
-      <c r="M157" s="40"/>
-      <c r="N157" s="81"/>
-      <c r="O157" s="40"/>
-      <c r="P157" s="153"/>
-      <c r="Q157" s="40"/>
-      <c r="R157" s="3"/>
-      <c r="S157" s="40"/>
-      <c r="T157" s="20"/>
-      <c r="U157" s="7"/>
-      <c r="V157" s="40"/>
-      <c r="W157" s="40"/>
-      <c r="X157" s="40"/>
-      <c r="Y157" s="40"/>
-      <c r="Z157" s="40"/>
-      <c r="AA157" s="35"/>
-      <c r="AC157" s="35"/>
-      <c r="AD157" s="2"/>
-      <c r="AE157" s="35"/>
-      <c r="AF157" s="35"/>
-      <c r="AG157" s="35"/>
-      <c r="AH157" s="35"/>
-      <c r="AI157" s="35"/>
-      <c r="AJ157" s="35"/>
-      <c r="AK157" s="35"/>
-      <c r="AL157" s="35"/>
-      <c r="AM157" s="35"/>
-      <c r="AN157" s="35"/>
-      <c r="AO157" s="35"/>
-      <c r="AP157" s="35"/>
-      <c r="AQ157" s="35"/>
-      <c r="AR157" s="35"/>
-      <c r="AS157" s="35"/>
-    </row>
-    <row r="158" spans="1:45" ht="13">
-      <c r="A158" s="40"/>
-      <c r="B158" s="40"/>
-      <c r="C158" s="40"/>
-      <c r="D158" s="7"/>
-      <c r="E158" s="40"/>
-      <c r="F158" s="40"/>
-      <c r="G158" s="40"/>
-      <c r="H158" s="40"/>
-      <c r="I158" s="40"/>
-      <c r="J158" s="40"/>
-      <c r="K158" s="40"/>
-      <c r="L158" s="40"/>
-      <c r="M158" s="40"/>
-      <c r="N158" s="81"/>
-      <c r="O158" s="40"/>
-      <c r="P158" s="153"/>
-      <c r="Q158" s="40"/>
-      <c r="R158" s="3"/>
-      <c r="S158" s="40"/>
-      <c r="T158" s="20"/>
-      <c r="U158" s="7"/>
-      <c r="V158" s="40"/>
-      <c r="W158" s="40"/>
-      <c r="X158" s="40"/>
-      <c r="Y158" s="40"/>
-      <c r="Z158" s="40"/>
-      <c r="AA158" s="35"/>
-      <c r="AC158" s="35"/>
-      <c r="AD158" s="2"/>
-      <c r="AE158" s="35"/>
-      <c r="AF158" s="35"/>
-      <c r="AG158" s="35"/>
-      <c r="AH158" s="35"/>
-      <c r="AI158" s="35"/>
-      <c r="AJ158" s="35"/>
-      <c r="AK158" s="35"/>
-      <c r="AL158" s="35"/>
-      <c r="AM158" s="35"/>
-      <c r="AN158" s="35"/>
-      <c r="AO158" s="35"/>
-      <c r="AP158" s="35"/>
-      <c r="AQ158" s="35"/>
-      <c r="AR158" s="35"/>
-      <c r="AS158" s="35"/>
+      <c r="A154" s="154">
+        <v>2017</v>
+      </c>
+      <c r="B154" s="154">
+        <v>8</v>
+      </c>
+      <c r="C154" s="154">
+        <v>31</v>
+      </c>
+      <c r="D154" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E154" s="170" t="s">
+        <v>420</v>
+      </c>
+      <c r="F154" s="170" t="s">
+        <v>1066</v>
+      </c>
+      <c r="G154" s="170" t="s">
+        <v>45</v>
+      </c>
+      <c r="H154" s="170" t="s">
+        <v>47</v>
+      </c>
+      <c r="I154" s="170" t="s">
+        <v>2061</v>
+      </c>
+      <c r="J154" s="170" t="s">
+        <v>2062</v>
+      </c>
+      <c r="K154" s="170"/>
+      <c r="L154" s="170" t="s">
+        <v>2063</v>
+      </c>
+      <c r="M154" s="170"/>
+      <c r="N154" s="171">
+        <v>147628</v>
+      </c>
+      <c r="O154" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="P154" s="170" t="s">
+        <v>2064</v>
+      </c>
+      <c r="Q154" s="170"/>
+      <c r="R154" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S154" s="170">
+        <v>3</v>
+      </c>
+      <c r="T154" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U154" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V154" s="172" t="s">
+        <v>2065</v>
+      </c>
+      <c r="W154" s="170" t="s">
+        <v>2066</v>
+      </c>
+      <c r="X154" s="170" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y154" s="170" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z154" s="170">
+        <v>110.5</v>
+      </c>
+      <c r="AA154" s="170" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB154" s="171">
+        <v>147628</v>
+      </c>
+      <c r="AC154" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD154" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE154" s="170"/>
+      <c r="AF154" s="170"/>
+      <c r="AG154" s="170"/>
+      <c r="AH154" s="170"/>
+      <c r="AI154" s="170"/>
+      <c r="AJ154" s="170"/>
+      <c r="AK154" s="170"/>
+      <c r="AL154" s="170"/>
+      <c r="AM154" s="170"/>
+      <c r="AN154" s="170"/>
+      <c r="AO154" s="170"/>
+      <c r="AP154" s="170"/>
+      <c r="AQ154" s="170"/>
+      <c r="AR154" s="170"/>
+      <c r="AS154" s="170"/>
+    </row>
+    <row r="155" spans="1:45" ht="19">
+      <c r="A155" s="154">
+        <v>2018</v>
+      </c>
+      <c r="B155" s="154">
+        <v>1</v>
+      </c>
+      <c r="C155" s="154">
+        <v>9</v>
+      </c>
+      <c r="D155" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E155" s="170" t="s">
+        <v>1715</v>
+      </c>
+      <c r="F155" s="170"/>
+      <c r="G155" s="170" t="s">
+        <v>45</v>
+      </c>
+      <c r="H155" s="170" t="s">
+        <v>2061</v>
+      </c>
+      <c r="I155" s="170"/>
+      <c r="J155" s="170" t="s">
+        <v>2053</v>
+      </c>
+      <c r="K155" s="170"/>
+      <c r="L155" s="170" t="s">
+        <v>2063</v>
+      </c>
+      <c r="M155" s="170"/>
+      <c r="N155" s="170"/>
+      <c r="O155" s="170"/>
+      <c r="P155" s="170"/>
+      <c r="Q155" s="170"/>
+      <c r="R155" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S155" s="170">
+        <v>1</v>
+      </c>
+      <c r="T155" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U155" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V155" s="172" t="s">
+        <v>2067</v>
+      </c>
+      <c r="W155" s="170"/>
+      <c r="X155" s="170" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y155" s="170" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z155" s="175">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="AA155" s="170" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB155" s="170"/>
+      <c r="AC155" s="170"/>
+      <c r="AD155" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE155" s="170"/>
+      <c r="AF155" s="170" t="s">
+        <v>2049</v>
+      </c>
+      <c r="AG155" s="170"/>
+      <c r="AH155" s="170"/>
+      <c r="AI155" s="170"/>
+      <c r="AJ155" s="170"/>
+      <c r="AK155" s="170"/>
+      <c r="AL155" s="170"/>
+      <c r="AM155" s="170"/>
+      <c r="AN155" s="170"/>
+      <c r="AO155" s="170"/>
+      <c r="AP155" s="170"/>
+      <c r="AQ155" s="170"/>
+      <c r="AR155" s="170"/>
+      <c r="AS155" s="170"/>
+    </row>
+    <row r="156" spans="1:45" ht="56">
+      <c r="A156" s="154">
+        <v>2015</v>
+      </c>
+      <c r="B156" s="154">
+        <v>4</v>
+      </c>
+      <c r="C156" s="154"/>
+      <c r="D156" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E156" s="170" t="s">
+        <v>420</v>
+      </c>
+      <c r="F156" s="170" t="s">
+        <v>1666</v>
+      </c>
+      <c r="G156" s="170" t="s">
+        <v>1980</v>
+      </c>
+      <c r="H156" s="170" t="s">
+        <v>2068</v>
+      </c>
+      <c r="I156" s="170" t="s">
+        <v>2069</v>
+      </c>
+      <c r="J156" s="170" t="s">
+        <v>2070</v>
+      </c>
+      <c r="K156" s="170"/>
+      <c r="L156" s="170"/>
+      <c r="M156" s="170"/>
+      <c r="N156" s="170"/>
+      <c r="O156" s="170"/>
+      <c r="P156" s="170"/>
+      <c r="Q156" s="170"/>
+      <c r="R156" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S156" s="170"/>
+      <c r="T156" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U156" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V156" s="172" t="s">
+        <v>2071</v>
+      </c>
+      <c r="W156" s="173" t="s">
+        <v>2072</v>
+      </c>
+      <c r="X156" s="170" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y156" s="170" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z156" s="170">
+        <v>378.5</v>
+      </c>
+      <c r="AA156" s="170" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB156" s="170"/>
+      <c r="AC156" s="170"/>
+      <c r="AD156" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE156" s="170"/>
+      <c r="AF156" s="170"/>
+      <c r="AG156" s="170"/>
+      <c r="AH156" s="170"/>
+      <c r="AI156" s="170"/>
+      <c r="AJ156" s="170"/>
+      <c r="AK156" s="170"/>
+      <c r="AL156" s="170"/>
+      <c r="AM156" s="170"/>
+      <c r="AN156" s="170"/>
+      <c r="AO156" s="170"/>
+      <c r="AP156" s="170"/>
+      <c r="AQ156" s="170"/>
+      <c r="AR156" s="170"/>
+      <c r="AS156" s="170"/>
+    </row>
+    <row r="157" spans="1:45" ht="28">
+      <c r="A157" s="154">
+        <v>2016</v>
+      </c>
+      <c r="B157" s="154">
+        <v>7</v>
+      </c>
+      <c r="C157" s="154">
+        <v>26</v>
+      </c>
+      <c r="D157" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E157" s="170" t="s">
+        <v>428</v>
+      </c>
+      <c r="F157" s="170" t="s">
+        <v>1228</v>
+      </c>
+      <c r="G157" s="173" t="s">
+        <v>1491</v>
+      </c>
+      <c r="H157" s="170" t="s">
+        <v>2073</v>
+      </c>
+      <c r="I157" s="170"/>
+      <c r="J157" s="170" t="s">
+        <v>2074</v>
+      </c>
+      <c r="K157" s="170"/>
+      <c r="L157" s="170" t="s">
+        <v>1662</v>
+      </c>
+      <c r="M157" s="170"/>
+      <c r="N157" s="171">
+        <v>3340</v>
+      </c>
+      <c r="O157" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="P157" s="170"/>
+      <c r="Q157" s="170"/>
+      <c r="R157" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S157" s="170"/>
+      <c r="T157" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U157" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V157" s="172" t="s">
+        <v>2075</v>
+      </c>
+      <c r="W157" s="170" t="s">
+        <v>2076</v>
+      </c>
+      <c r="X157" s="170" t="s">
+        <v>260</v>
+      </c>
+      <c r="Y157" s="170"/>
+      <c r="Z157" s="170">
+        <v>2</v>
+      </c>
+      <c r="AA157" s="170" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB157" s="171">
+        <v>3340</v>
+      </c>
+      <c r="AC157" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD157" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE157" s="170"/>
+      <c r="AF157" s="170"/>
+      <c r="AG157" s="170"/>
+      <c r="AH157" s="170"/>
+      <c r="AI157" s="170"/>
+      <c r="AJ157" s="170"/>
+      <c r="AK157" s="170"/>
+      <c r="AL157" s="170"/>
+      <c r="AM157" s="170"/>
+      <c r="AN157" s="170"/>
+      <c r="AO157" s="170"/>
+      <c r="AP157" s="170"/>
+      <c r="AQ157" s="170"/>
+      <c r="AR157" s="170"/>
+      <c r="AS157" s="170"/>
+    </row>
+    <row r="158" spans="1:45" ht="28">
+      <c r="A158" s="154">
+        <v>2016</v>
+      </c>
+      <c r="B158" s="154">
+        <v>7</v>
+      </c>
+      <c r="C158" s="154">
+        <v>15</v>
+      </c>
+      <c r="D158" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E158" s="170" t="s">
+        <v>428</v>
+      </c>
+      <c r="F158" s="170" t="s">
+        <v>1504</v>
+      </c>
+      <c r="G158" s="170" t="s">
+        <v>1980</v>
+      </c>
+      <c r="H158" s="170" t="s">
+        <v>2077</v>
+      </c>
+      <c r="I158" s="170"/>
+      <c r="J158" s="170" t="s">
+        <v>2078</v>
+      </c>
+      <c r="K158" s="170"/>
+      <c r="L158" s="170" t="s">
+        <v>1662</v>
+      </c>
+      <c r="M158" s="170"/>
+      <c r="N158" s="171">
+        <v>19896</v>
+      </c>
+      <c r="O158" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="P158" s="170"/>
+      <c r="Q158" s="170"/>
+      <c r="R158" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S158" s="170"/>
+      <c r="T158" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U158" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V158" s="172" t="s">
+        <v>2079</v>
+      </c>
+      <c r="W158" s="170"/>
+      <c r="X158" s="173" t="s">
+        <v>1745</v>
+      </c>
+      <c r="Y158" s="173" t="s">
+        <v>1746</v>
+      </c>
+      <c r="Z158" s="173" t="s">
+        <v>2080</v>
+      </c>
+      <c r="AA158" s="170" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB158" s="171">
+        <v>4517</v>
+      </c>
+      <c r="AC158" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD158" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE158" s="170"/>
+      <c r="AF158" s="170" t="s">
+        <v>2049</v>
+      </c>
+      <c r="AG158" s="170"/>
+      <c r="AH158" s="170"/>
+      <c r="AI158" s="170"/>
+      <c r="AJ158" s="170"/>
+      <c r="AK158" s="170"/>
+      <c r="AL158" s="170"/>
+      <c r="AM158" s="170"/>
+      <c r="AN158" s="170"/>
+      <c r="AO158" s="170"/>
+      <c r="AP158" s="170"/>
+      <c r="AQ158" s="170"/>
+      <c r="AR158" s="170"/>
+      <c r="AS158" s="170"/>
     </row>
     <row r="159" spans="1:45" ht="13">
-      <c r="A159" s="40"/>
-      <c r="B159" s="40"/>
-      <c r="C159" s="40"/>
-      <c r="D159" s="7"/>
-      <c r="E159" s="40"/>
-      <c r="F159" s="40"/>
-      <c r="G159" s="40"/>
-      <c r="H159" s="40"/>
-      <c r="I159" s="40"/>
-      <c r="J159" s="40"/>
-      <c r="K159" s="40"/>
-      <c r="L159" s="40"/>
-      <c r="M159" s="40"/>
-      <c r="N159" s="81"/>
-      <c r="O159" s="40"/>
-      <c r="P159" s="153"/>
-      <c r="Q159" s="40"/>
-      <c r="R159" s="3"/>
-      <c r="S159" s="40"/>
-      <c r="T159" s="20"/>
-      <c r="U159" s="7"/>
-      <c r="V159" s="40"/>
-      <c r="W159" s="40"/>
-      <c r="X159" s="40"/>
-      <c r="Y159" s="40"/>
-      <c r="Z159" s="40"/>
-      <c r="AA159" s="35"/>
-      <c r="AC159" s="35"/>
-      <c r="AD159" s="2"/>
-      <c r="AE159" s="35"/>
-      <c r="AF159" s="35"/>
-      <c r="AG159" s="35"/>
-      <c r="AH159" s="35"/>
-      <c r="AI159" s="35"/>
-      <c r="AJ159" s="35"/>
-      <c r="AK159" s="35"/>
-      <c r="AL159" s="35"/>
-      <c r="AM159" s="35"/>
-      <c r="AN159" s="35"/>
-      <c r="AO159" s="35"/>
-      <c r="AP159" s="35"/>
-      <c r="AQ159" s="35"/>
-      <c r="AR159" s="35"/>
-      <c r="AS159" s="35"/>
-    </row>
-    <row r="160" spans="1:45" ht="13">
-      <c r="A160" s="40"/>
-      <c r="B160" s="40"/>
-      <c r="C160" s="40"/>
-      <c r="D160" s="7"/>
-      <c r="E160" s="40"/>
-      <c r="F160" s="40"/>
-      <c r="G160" s="40"/>
-      <c r="H160" s="40"/>
-      <c r="I160" s="40"/>
-      <c r="J160" s="40"/>
-      <c r="K160" s="40"/>
-      <c r="L160" s="40"/>
-      <c r="M160" s="40"/>
-      <c r="N160" s="81"/>
-      <c r="O160" s="40"/>
-      <c r="P160" s="153"/>
-      <c r="Q160" s="40"/>
-      <c r="R160" s="3"/>
-      <c r="S160" s="40"/>
-      <c r="T160" s="20"/>
-      <c r="U160" s="7"/>
-      <c r="V160" s="40"/>
-      <c r="W160" s="40"/>
-      <c r="X160" s="40"/>
-      <c r="Y160" s="40"/>
-      <c r="Z160" s="40"/>
-      <c r="AA160" s="35"/>
-      <c r="AC160" s="35"/>
-      <c r="AD160" s="2"/>
-      <c r="AE160" s="35"/>
-      <c r="AF160" s="35"/>
-      <c r="AG160" s="35"/>
-      <c r="AH160" s="35"/>
-      <c r="AI160" s="35"/>
-      <c r="AJ160" s="35"/>
-      <c r="AK160" s="35"/>
-      <c r="AL160" s="35"/>
-      <c r="AM160" s="35"/>
-      <c r="AN160" s="35"/>
-      <c r="AO160" s="35"/>
-      <c r="AP160" s="35"/>
-      <c r="AQ160" s="35"/>
-      <c r="AR160" s="35"/>
-      <c r="AS160" s="35"/>
+      <c r="A159" s="154">
+        <v>2016</v>
+      </c>
+      <c r="B159" s="154">
+        <v>10</v>
+      </c>
+      <c r="C159" s="154">
+        <v>25</v>
+      </c>
+      <c r="D159" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E159" s="170" t="s">
+        <v>428</v>
+      </c>
+      <c r="F159" s="170" t="s">
+        <v>1228</v>
+      </c>
+      <c r="G159" s="170" t="s">
+        <v>1980</v>
+      </c>
+      <c r="H159" s="170" t="s">
+        <v>2073</v>
+      </c>
+      <c r="I159" s="170"/>
+      <c r="J159" s="170" t="s">
+        <v>2074</v>
+      </c>
+      <c r="K159" s="170"/>
+      <c r="L159" s="170"/>
+      <c r="M159" s="170"/>
+      <c r="N159" s="171">
+        <v>22712</v>
+      </c>
+      <c r="O159" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="P159" s="170"/>
+      <c r="Q159" s="170"/>
+      <c r="R159" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S159" s="170"/>
+      <c r="T159" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U159" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V159" s="172" t="s">
+        <v>2081</v>
+      </c>
+      <c r="W159" s="170"/>
+      <c r="X159" s="170" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y159" s="170" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z159" s="170">
+        <v>7924</v>
+      </c>
+      <c r="AA159" s="170" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB159" s="171">
+        <v>22712</v>
+      </c>
+      <c r="AC159" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD159" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE159" s="170"/>
+      <c r="AF159" s="170"/>
+      <c r="AG159" s="170"/>
+      <c r="AH159" s="170"/>
+      <c r="AI159" s="170"/>
+      <c r="AJ159" s="170"/>
+      <c r="AK159" s="170"/>
+      <c r="AL159" s="170"/>
+      <c r="AM159" s="170"/>
+      <c r="AN159" s="170"/>
+      <c r="AO159" s="170"/>
+      <c r="AP159" s="170"/>
+      <c r="AQ159" s="170"/>
+      <c r="AR159" s="170"/>
+      <c r="AS159" s="170"/>
+    </row>
+    <row r="160" spans="1:45" ht="14">
+      <c r="A160" s="154">
+        <v>2016</v>
+      </c>
+      <c r="B160" s="154">
+        <v>12</v>
+      </c>
+      <c r="C160" s="154">
+        <v>5</v>
+      </c>
+      <c r="D160" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E160" s="170" t="s">
+        <v>428</v>
+      </c>
+      <c r="F160" s="170" t="s">
+        <v>1228</v>
+      </c>
+      <c r="G160" s="170" t="s">
+        <v>45</v>
+      </c>
+      <c r="H160" s="170" t="s">
+        <v>2073</v>
+      </c>
+      <c r="I160" s="170" t="s">
+        <v>2074</v>
+      </c>
+      <c r="J160" s="170" t="s">
+        <v>2082</v>
+      </c>
+      <c r="K160" s="170"/>
+      <c r="L160" s="170" t="s">
+        <v>1679</v>
+      </c>
+      <c r="M160" s="170"/>
+      <c r="N160" s="171">
+        <v>14696</v>
+      </c>
+      <c r="O160" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="P160" s="170"/>
+      <c r="Q160" s="170"/>
+      <c r="R160" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S160" s="170"/>
+      <c r="T160" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U160" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V160" s="172" t="s">
+        <v>2083</v>
+      </c>
+      <c r="W160" s="176" t="s">
+        <v>1301</v>
+      </c>
+      <c r="X160" s="170" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y160" s="170" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z160" s="170">
+        <v>5886</v>
+      </c>
+      <c r="AA160" s="170" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB160" s="171">
+        <v>14696</v>
+      </c>
+      <c r="AC160" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD160" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE160" s="170"/>
+      <c r="AF160" s="170"/>
+      <c r="AG160" s="170"/>
+      <c r="AH160" s="170"/>
+      <c r="AI160" s="170"/>
+      <c r="AJ160" s="170"/>
+      <c r="AK160" s="170"/>
+      <c r="AL160" s="170"/>
+      <c r="AM160" s="170"/>
+      <c r="AN160" s="170"/>
+      <c r="AO160" s="170"/>
+      <c r="AP160" s="170"/>
+      <c r="AQ160" s="170"/>
+      <c r="AR160" s="170"/>
+      <c r="AS160" s="170"/>
     </row>
     <row r="161" spans="1:45" ht="13">
-      <c r="A161" s="40"/>
-      <c r="B161" s="40"/>
-      <c r="C161" s="40"/>
-      <c r="D161" s="7"/>
-      <c r="E161" s="40"/>
-      <c r="F161" s="40"/>
-      <c r="G161" s="40"/>
-      <c r="H161" s="40"/>
-      <c r="I161" s="40"/>
-      <c r="J161" s="40"/>
-      <c r="K161" s="40"/>
-      <c r="L161" s="40"/>
-      <c r="M161" s="40"/>
-      <c r="N161" s="81"/>
-      <c r="O161" s="40"/>
-      <c r="P161" s="153"/>
-      <c r="Q161" s="40"/>
-      <c r="R161" s="3"/>
-      <c r="S161" s="40"/>
-      <c r="T161" s="20"/>
-      <c r="U161" s="7"/>
-      <c r="V161" s="40"/>
-      <c r="W161" s="40"/>
-      <c r="X161" s="40"/>
-      <c r="Y161" s="40"/>
-      <c r="Z161" s="40"/>
-      <c r="AA161" s="35"/>
-      <c r="AC161" s="35"/>
-      <c r="AD161" s="2"/>
-      <c r="AE161" s="35"/>
-      <c r="AF161" s="35"/>
-      <c r="AG161" s="35"/>
-      <c r="AH161" s="35"/>
-      <c r="AI161" s="35"/>
-      <c r="AJ161" s="35"/>
-      <c r="AK161" s="35"/>
-      <c r="AL161" s="35"/>
-      <c r="AM161" s="35"/>
-      <c r="AN161" s="35"/>
-      <c r="AO161" s="35"/>
-      <c r="AP161" s="35"/>
-      <c r="AQ161" s="35"/>
-      <c r="AR161" s="35"/>
-      <c r="AS161" s="35"/>
+      <c r="A161" s="154">
+        <v>2016</v>
+      </c>
+      <c r="B161" s="154">
+        <v>8</v>
+      </c>
+      <c r="C161" s="154">
+        <v>3</v>
+      </c>
+      <c r="D161" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E161" s="170" t="s">
+        <v>428</v>
+      </c>
+      <c r="F161" s="170" t="s">
+        <v>1462</v>
+      </c>
+      <c r="G161" s="170" t="s">
+        <v>1980</v>
+      </c>
+      <c r="H161" s="170"/>
+      <c r="I161" s="170"/>
+      <c r="J161" s="170"/>
+      <c r="K161" s="170"/>
+      <c r="L161" s="170" t="s">
+        <v>1662</v>
+      </c>
+      <c r="M161" s="170"/>
+      <c r="N161" s="171">
+        <v>14696</v>
+      </c>
+      <c r="O161" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="P161" s="170"/>
+      <c r="Q161" s="170"/>
+      <c r="R161" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S161" s="170"/>
+      <c r="T161" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U161" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V161" s="172" t="s">
+        <v>2084</v>
+      </c>
+      <c r="W161" s="170"/>
+      <c r="X161" s="170" t="s">
+        <v>260</v>
+      </c>
+      <c r="Y161" s="170"/>
+      <c r="Z161" s="170">
+        <v>4</v>
+      </c>
+      <c r="AA161" s="170" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB161" s="171">
+        <v>6680</v>
+      </c>
+      <c r="AC161" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD161" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE161" s="170"/>
+      <c r="AF161" s="170" t="s">
+        <v>2049</v>
+      </c>
+      <c r="AG161" s="170"/>
+      <c r="AH161" s="170"/>
+      <c r="AI161" s="170"/>
+      <c r="AJ161" s="170"/>
+      <c r="AK161" s="170"/>
+      <c r="AL161" s="170"/>
+      <c r="AM161" s="170"/>
+      <c r="AN161" s="170"/>
+      <c r="AO161" s="170"/>
+      <c r="AP161" s="170"/>
+      <c r="AQ161" s="170"/>
+      <c r="AR161" s="170"/>
+      <c r="AS161" s="170"/>
     </row>
     <row r="162" spans="1:45" ht="13">
-      <c r="A162" s="40"/>
-      <c r="B162" s="40"/>
-      <c r="C162" s="40"/>
-      <c r="D162" s="7"/>
-      <c r="E162" s="40"/>
-      <c r="F162" s="40"/>
-      <c r="G162" s="40"/>
-      <c r="H162" s="40"/>
-      <c r="I162" s="40"/>
-      <c r="J162" s="40"/>
-      <c r="K162" s="40"/>
-      <c r="L162" s="40"/>
-      <c r="M162" s="40"/>
-      <c r="N162" s="81"/>
-      <c r="O162" s="40"/>
-      <c r="P162" s="153"/>
-      <c r="Q162" s="40"/>
-      <c r="R162" s="3"/>
-      <c r="S162" s="40"/>
-      <c r="T162" s="20"/>
-      <c r="U162" s="7"/>
-      <c r="V162" s="40"/>
-      <c r="W162" s="40"/>
-      <c r="X162" s="40"/>
-      <c r="Y162" s="40"/>
-      <c r="Z162" s="40"/>
-      <c r="AA162" s="35"/>
-      <c r="AC162" s="35"/>
-      <c r="AD162" s="2"/>
-      <c r="AE162" s="35"/>
-      <c r="AF162" s="35"/>
-      <c r="AG162" s="35"/>
-      <c r="AH162" s="35"/>
-      <c r="AI162" s="35"/>
-      <c r="AJ162" s="35"/>
-      <c r="AK162" s="35"/>
-      <c r="AL162" s="35"/>
-      <c r="AM162" s="35"/>
-      <c r="AN162" s="35"/>
-      <c r="AO162" s="35"/>
-      <c r="AP162" s="35"/>
-      <c r="AQ162" s="35"/>
-      <c r="AR162" s="35"/>
-      <c r="AS162" s="35"/>
-    </row>
-    <row r="163" spans="1:45" ht="13">
-      <c r="A163" s="40"/>
-      <c r="B163" s="40"/>
-      <c r="C163" s="40"/>
-      <c r="D163" s="7"/>
-      <c r="E163" s="40"/>
-      <c r="F163" s="40"/>
-      <c r="G163" s="40"/>
-      <c r="H163" s="40"/>
-      <c r="I163" s="40"/>
-      <c r="J163" s="40"/>
-      <c r="K163" s="40"/>
-      <c r="L163" s="40"/>
-      <c r="M163" s="40"/>
-      <c r="N163" s="81"/>
-      <c r="O163" s="40"/>
-      <c r="P163" s="153"/>
-      <c r="Q163" s="40"/>
-      <c r="R163" s="3"/>
-      <c r="S163" s="40"/>
-      <c r="T163" s="20"/>
-      <c r="U163" s="7"/>
-      <c r="V163" s="40"/>
-      <c r="W163" s="40"/>
-      <c r="X163" s="40"/>
-      <c r="Y163" s="40"/>
-      <c r="Z163" s="40"/>
-      <c r="AA163" s="35"/>
-      <c r="AC163" s="35"/>
-      <c r="AD163" s="2"/>
-      <c r="AE163" s="35"/>
-      <c r="AF163" s="35"/>
-      <c r="AG163" s="35"/>
-      <c r="AH163" s="35"/>
-      <c r="AI163" s="35"/>
-      <c r="AJ163" s="35"/>
-      <c r="AK163" s="35"/>
-      <c r="AL163" s="35"/>
-      <c r="AM163" s="35"/>
-      <c r="AN163" s="35"/>
-      <c r="AO163" s="35"/>
-      <c r="AP163" s="35"/>
-      <c r="AQ163" s="35"/>
-      <c r="AR163" s="35"/>
-      <c r="AS163" s="35"/>
+      <c r="A162" s="154">
+        <v>2016</v>
+      </c>
+      <c r="B162" s="154">
+        <v>10</v>
+      </c>
+      <c r="C162" s="154">
+        <v>2</v>
+      </c>
+      <c r="D162" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E162" s="170" t="s">
+        <v>428</v>
+      </c>
+      <c r="F162" s="170" t="s">
+        <v>1228</v>
+      </c>
+      <c r="G162" s="170" t="s">
+        <v>45</v>
+      </c>
+      <c r="H162" s="170" t="s">
+        <v>2073</v>
+      </c>
+      <c r="I162" s="170"/>
+      <c r="J162" s="170" t="s">
+        <v>2074</v>
+      </c>
+      <c r="K162" s="170"/>
+      <c r="L162" s="170" t="s">
+        <v>1850</v>
+      </c>
+      <c r="M162" s="170"/>
+      <c r="N162" s="171">
+        <v>22635</v>
+      </c>
+      <c r="O162" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="P162" s="170"/>
+      <c r="Q162" s="170"/>
+      <c r="R162" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S162" s="170"/>
+      <c r="T162" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U162" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V162" s="172" t="s">
+        <v>2085</v>
+      </c>
+      <c r="W162" s="170"/>
+      <c r="X162" s="170" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y162" s="170" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z162" s="170">
+        <v>6302</v>
+      </c>
+      <c r="AA162" s="170" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB162" s="171">
+        <v>18704</v>
+      </c>
+      <c r="AC162" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD162" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE162" s="170"/>
+      <c r="AF162" s="170" t="s">
+        <v>2086</v>
+      </c>
+      <c r="AG162" s="170"/>
+      <c r="AH162" s="170"/>
+      <c r="AI162" s="170"/>
+      <c r="AJ162" s="170"/>
+      <c r="AK162" s="170"/>
+      <c r="AL162" s="170"/>
+      <c r="AM162" s="170"/>
+      <c r="AN162" s="170"/>
+      <c r="AO162" s="170"/>
+      <c r="AP162" s="170"/>
+      <c r="AQ162" s="170"/>
+      <c r="AR162" s="170"/>
+      <c r="AS162" s="170"/>
+    </row>
+    <row r="163" spans="1:45" ht="42">
+      <c r="A163" s="154">
+        <v>2017</v>
+      </c>
+      <c r="B163" s="154">
+        <v>4</v>
+      </c>
+      <c r="C163" s="154">
+        <v>17</v>
+      </c>
+      <c r="D163" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="E163" s="170" t="s">
+        <v>2087</v>
+      </c>
+      <c r="F163" s="170" t="s">
+        <v>2088</v>
+      </c>
+      <c r="G163" s="173" t="s">
+        <v>430</v>
+      </c>
+      <c r="H163" s="170"/>
+      <c r="I163" s="170"/>
+      <c r="J163" s="170"/>
+      <c r="K163" s="170"/>
+      <c r="L163" s="170"/>
+      <c r="M163" s="170"/>
+      <c r="N163" s="171">
+        <v>55110</v>
+      </c>
+      <c r="O163" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="P163" s="170"/>
+      <c r="Q163" s="170"/>
+      <c r="R163" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="S163" s="170"/>
+      <c r="T163" s="170" t="s">
+        <v>107</v>
+      </c>
+      <c r="U163" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="V163" s="172" t="s">
+        <v>2089</v>
+      </c>
+      <c r="W163" s="170"/>
+      <c r="X163" s="170" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y163" s="170" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z163" s="170">
+        <v>13105.5</v>
+      </c>
+      <c r="AA163" s="170" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB163" s="171">
+        <v>55110</v>
+      </c>
+      <c r="AC163" s="170" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD163" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE163" s="170"/>
+      <c r="AF163" s="170" t="s">
+        <v>2090</v>
+      </c>
+      <c r="AG163" s="170"/>
+      <c r="AH163" s="170"/>
+      <c r="AI163" s="170"/>
+      <c r="AJ163" s="170"/>
+      <c r="AK163" s="170"/>
+      <c r="AL163" s="170"/>
+      <c r="AM163" s="170"/>
+      <c r="AN163" s="170"/>
+      <c r="AO163" s="170"/>
+      <c r="AP163" s="170"/>
+      <c r="AQ163" s="170"/>
+      <c r="AR163" s="170"/>
+      <c r="AS163" s="170"/>
     </row>
     <row r="164" spans="1:45" ht="13">
       <c r="A164" s="40"/>
@@ -60117,9 +61216,27 @@
     <hyperlink ref="V143" r:id="rId136" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
     <hyperlink ref="V144" r:id="rId137" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
     <hyperlink ref="V145" r:id="rId138" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="V146" r:id="rId139" xr:uid="{9213AE93-B9DC-9840-B448-043E3C1D4357}"/>
+    <hyperlink ref="V147" r:id="rId140" display="https://www.itslaw.com/detail?judgementId=f1dd42a3-8e14-4a59-ae91-027232b86184&amp;area=0&amp;index=9&amp;sortType=2&amp;count=20&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2019%2B7%2B2019" xr:uid="{29F4685B-71AD-FD48-A788-13A26CCA3703}"/>
+    <hyperlink ref="V148" r:id="rId141" display="https://www.itslaw.com/detail?judgementId=af840564-ec8a-4674-8f78-2243a65f3310&amp;area=0&amp;index=5&amp;sortType=2&amp;count=20&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2019%2B7%2B2019" xr:uid="{25E56DA7-8F3C-BF43-8EF6-EE23DC916AB9}"/>
+    <hyperlink ref="V149" r:id="rId142" display="https://www.itslaw.com/detail?judgementId=0f816eb5-7e64-4b2f-a4c3-a65eefcdb33c&amp;area=0&amp;index=119&amp;sortType=2&amp;count=120&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2018%2B7%2B2018" xr:uid="{6E9F3D55-A714-F24C-B4B2-1C1A0F8E2ECB}"/>
+    <hyperlink ref="V150" r:id="rId143" display="https://www.itslaw.com/detail?judgementId=370b1547-85ae-4d83-ad1e-8c05e3380bd4&amp;area=0&amp;index=100&amp;sortType=2&amp;count=120&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2018%2B7%2B2018" xr:uid="{B7C42C1A-CB1B-6347-913E-7F4A960AA965}"/>
+    <hyperlink ref="V151" r:id="rId144" display="https://www.itslaw.com/detail?judgementId=a94a9e50-0d56-4017-b1cb-e154aa783369&amp;area=0&amp;index=94&amp;sortType=2&amp;count=120&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2018%2B7%2B2018" xr:uid="{7490BAA4-AB6F-E642-B000-347BE258E4B5}"/>
+    <hyperlink ref="V152" r:id="rId145" display="https://www.itslaw.com/detail?judgementId=95a5f1f7-17e3-4273-9bc8-e5d5198a359c&amp;area=0&amp;index=92&amp;sortType=2&amp;count=120&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2018%2B7%2B2018" xr:uid="{07E66647-09B5-2943-AFB2-D1DA3639067E}"/>
+    <hyperlink ref="V153" r:id="rId146" display="https://www.itslaw.com/detail?judgementId=b0fed416-ebf4-49a1-9a1a-8845bbb34e37&amp;area=0&amp;index=87&amp;sortType=2&amp;count=120&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2018%2B7%2B2018" xr:uid="{6C347811-097A-424E-A832-C4C50B4FB89B}"/>
+    <hyperlink ref="V154" r:id="rId147" display="https://www.itslaw.com/detail?judgementId=56658deb-0901-4c3c-b0f2-f37098878b5b&amp;area=0&amp;index=78&amp;sortType=2&amp;count=120&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2018%2B7%2B2018" xr:uid="{9854FC0A-7F1B-AE49-AA03-41099F6528BE}"/>
+    <hyperlink ref="V155" r:id="rId148" display="https://www.itslaw.com/detail?judgementId=750edd50-d798-4804-b1f8-24c7ae107c33&amp;area=0&amp;index=16&amp;sortType=2&amp;count=120&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2018%2B7%2B2018" xr:uid="{ABD0C43D-C586-1249-8AB4-E0A4D904C900}"/>
+    <hyperlink ref="V156" r:id="rId149" display="https://www.itslaw.com/detail?judgementId=1f94f63e-146b-4715-9c9d-d704126c8506&amp;area=0&amp;index=3&amp;sortType=2&amp;count=120&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2018%2B7%2B2018" xr:uid="{E87CD80B-7B72-0146-B096-C5F6A7E0DD3D}"/>
+    <hyperlink ref="V157" r:id="rId150" display="https://www.itslaw.com/detail?judgementId=56172897-68e4-4a17-85f7-c845792aa1f3&amp;area=0&amp;index=100&amp;sortType=2&amp;count=101&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2017%2B7%2B2017" xr:uid="{B7F1E6E6-0E47-474E-A850-FECB8C8B3638}"/>
+    <hyperlink ref="V158" r:id="rId151" display="https://www.itslaw.com/detail?judgementId=97dc8373-005f-42e3-a988-ef582e54ce9a&amp;area=0&amp;index=98&amp;sortType=2&amp;count=101&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2017%2B7%2B2017" xr:uid="{5C87ECF2-9DD1-284B-90B9-8EFE81EC0636}"/>
+    <hyperlink ref="V159" r:id="rId152" display="https://www.itslaw.com/detail?judgementId=b573442b-55b0-4f2c-9b75-e17faa4c2dd1&amp;area=0&amp;index=68&amp;sortType=2&amp;count=101&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2017%2B7%2B2017" xr:uid="{BAAE9267-43A8-5C47-9B26-663195120A30}"/>
+    <hyperlink ref="V160" r:id="rId153" display="https://www.itslaw.com/detail?judgementId=914deead-897f-4324-8665-929402616f0f&amp;area=0&amp;index=47&amp;sortType=2&amp;count=101&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2017%2B7%2B2017" xr:uid="{37DB1906-F788-2A4E-9DD8-0017FD12004C}"/>
+    <hyperlink ref="V161" r:id="rId154" display="https://www.itslaw.com/detail?judgementId=479efecc-6f48-4072-81cb-db013c515105&amp;area=0&amp;index=41&amp;sortType=2&amp;count=101&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2017%2B7%2B2017" xr:uid="{041DB140-1652-1C4E-B615-9B43201C823D}"/>
+    <hyperlink ref="V162" r:id="rId155" display="https://www.itslaw.com/detail?judgementId=a3c83d7d-4184-4a8c-8ecc-8118b1c9d5c6&amp;area=0&amp;index=28&amp;sortType=2&amp;count=101&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2017%2B7%2B2017" xr:uid="{44FAB309-B5B3-3647-8A7B-ACA9341CE57F}"/>
+    <hyperlink ref="V163" r:id="rId156" display="https://www.itslaw.com/detail?judgementId=b387494a-27c4-44d2-8f87-bc3f9226a67f&amp;area=0&amp;index=18&amp;sortType=2&amp;count=101&amp;conditions=searchWord%2B%E7%A9%BF%E5%B1%B1%E7%94%B2%2B1%2B%E7%A9%BF%E5%B1%B1%E7%94%B2&amp;conditions=caseType%2B2%2B10%2B%E5%88%91%E4%BA%8B&amp;conditions=trialYear%2B2017%2B7%2B2017" xr:uid="{53021D2C-5267-DE42-9DAA-61DCCEBB6838}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId139"/>
+  <legacyDrawing r:id="rId157"/>
 </worksheet>
 </file>
 
@@ -60156,7 +61273,7 @@
       <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A2" s="162" t="s">
+      <c r="A2" s="168" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -60170,7 +61287,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A3" s="160"/>
+      <c r="A3" s="166"/>
       <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
@@ -60182,7 +61299,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A4" s="160"/>
+      <c r="A4" s="166"/>
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -60194,7 +61311,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A5" s="160"/>
+      <c r="A5" s="166"/>
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
@@ -60206,7 +61323,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A6" s="160"/>
+      <c r="A6" s="166"/>
       <c r="B6" s="9" t="s">
         <v>86</v>
       </c>
@@ -60216,7 +61333,7 @@
       <c r="D6" s="17"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A7" s="160"/>
+      <c r="A7" s="166"/>
       <c r="B7" s="9" t="s">
         <v>5</v>
       </c>
@@ -60226,7 +61343,7 @@
       <c r="D7" s="17"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A8" s="160"/>
+      <c r="A8" s="166"/>
       <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
@@ -60238,7 +61355,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A9" s="160"/>
+      <c r="A9" s="166"/>
       <c r="B9" s="9" t="s">
         <v>7</v>
       </c>
@@ -60250,7 +61367,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A10" s="160"/>
+      <c r="A10" s="166"/>
       <c r="B10" s="9" t="s">
         <v>8</v>
       </c>
@@ -60262,7 +61379,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A11" s="160"/>
+      <c r="A11" s="166"/>
       <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
@@ -60274,7 +61391,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A12" s="160"/>
+      <c r="A12" s="166"/>
       <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
@@ -60286,7 +61403,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A13" s="160"/>
+      <c r="A13" s="166"/>
       <c r="B13" s="9" t="s">
         <v>11</v>
       </c>
@@ -60296,7 +61413,7 @@
       <c r="D13" s="17"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A14" s="160"/>
+      <c r="A14" s="166"/>
       <c r="B14" s="9" t="s">
         <v>12</v>
       </c>
@@ -60306,7 +61423,7 @@
       <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A15" s="160"/>
+      <c r="A15" s="166"/>
       <c r="B15" s="9" t="s">
         <v>128</v>
       </c>
@@ -60319,7 +61436,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A16" s="160"/>
+      <c r="A16" s="166"/>
       <c r="B16" s="9" t="s">
         <v>17</v>
       </c>
@@ -60332,7 +61449,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A17" s="160"/>
+      <c r="A17" s="166"/>
       <c r="B17" s="9" t="s">
         <v>18</v>
       </c>
@@ -60347,7 +61464,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A18" s="160"/>
+      <c r="A18" s="166"/>
       <c r="B18" s="9" t="s">
         <v>20</v>
       </c>
@@ -60357,7 +61474,7 @@
       <c r="D18" s="17"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A19" s="160"/>
+      <c r="A19" s="166"/>
       <c r="B19" s="9" t="s">
         <v>25</v>
       </c>
@@ -60367,7 +61484,7 @@
       <c r="D19" s="17"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A20" s="160"/>
+      <c r="A20" s="166"/>
       <c r="B20" s="9" t="s">
         <v>26</v>
       </c>
@@ -60377,7 +61494,7 @@
       <c r="D20" s="17"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A21" s="160"/>
+      <c r="A21" s="166"/>
       <c r="B21" s="9" t="s">
         <v>154</v>
       </c>
@@ -60392,7 +61509,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A22" s="160"/>
+      <c r="A22" s="166"/>
       <c r="B22" s="9" t="s">
         <v>27</v>
       </c>
@@ -60402,7 +61519,7 @@
       <c r="D22" s="17"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A23" s="160"/>
+      <c r="A23" s="166"/>
       <c r="B23" s="9" t="s">
         <v>28</v>
       </c>
@@ -60412,7 +61529,7 @@
       <c r="D23" s="17"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A24" s="160"/>
+      <c r="A24" s="166"/>
       <c r="B24" s="9" t="s">
         <v>29</v>
       </c>
@@ -60422,7 +61539,7 @@
       <c r="D24" s="17"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A25" s="162" t="s">
+      <c r="A25" s="168" t="s">
         <v>176</v>
       </c>
       <c r="B25" s="9" t="s">
@@ -60436,7 +61553,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A26" s="160"/>
+      <c r="A26" s="166"/>
       <c r="B26" s="9" t="s">
         <v>181</v>
       </c>
@@ -60448,7 +61565,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A27" s="160"/>
+      <c r="A27" s="166"/>
       <c r="B27" s="9" t="s">
         <v>32</v>
       </c>
@@ -60463,7 +61580,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A28" s="160"/>
+      <c r="A28" s="166"/>
       <c r="B28" s="9" t="s">
         <v>33</v>
       </c>
@@ -60475,7 +61592,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A29" s="160"/>
+      <c r="A29" s="166"/>
       <c r="B29" s="9" t="s">
         <v>34</v>
       </c>
@@ -60487,7 +61604,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A30" s="160"/>
+      <c r="A30" s="166"/>
       <c r="B30" s="9" t="s">
         <v>128</v>
       </c>
@@ -60500,7 +61617,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A31" s="160"/>
+      <c r="A31" s="166"/>
       <c r="B31" s="9" t="s">
         <v>17</v>
       </c>
@@ -60513,7 +61630,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A32" s="162" t="s">
+      <c r="A32" s="168" t="s">
         <v>218</v>
       </c>
       <c r="B32" s="9" t="s">
@@ -60527,7 +61644,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A33" s="160"/>
+      <c r="A33" s="166"/>
       <c r="B33" s="9" t="s">
         <v>37</v>
       </c>
@@ -60539,7 +61656,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A34" s="160"/>
+      <c r="A34" s="166"/>
       <c r="B34" s="9" t="s">
         <v>38</v>
       </c>
@@ -60558,18 +61675,18 @@
       <c r="A36" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B36" s="159" t="s">
+      <c r="B36" s="165" t="s">
         <v>283</v>
       </c>
-      <c r="C36" s="160"/>
-      <c r="D36" s="160"/>
+      <c r="C36" s="166"/>
+      <c r="D36" s="166"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1">
-      <c r="B37" s="161" t="s">
+      <c r="B37" s="167" t="s">
         <v>294</v>
       </c>
-      <c r="C37" s="160"/>
-      <c r="D37" s="160"/>
+      <c r="C37" s="166"/>
+      <c r="D37" s="166"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1">
       <c r="B38" s="9"/>
@@ -71792,10 +72909,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="169" t="s">
         <v>1435</v>
       </c>
-      <c r="B1" s="160"/>
+      <c r="B1" s="166"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="94" t="s">

</xml_diff>